<commit_message>
After database reorg and table creation from airr schema
</commit_message>
<xml_diff>
--- a/db/airr_schema_defs.xlsx
+++ b/db/airr_schema_defs.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,14 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Research\digby_backend\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{D47DD5FF-3530-4EF1-9251-4DC17A352B8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5BECAD40-870A-42C2-B9E4-88AAA35DB73B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="airr_schema_defs" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1791,7 +1803,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2637,11 +2649,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="H135" sqref="H135"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5183,6 +5195,9 @@
       <c r="D90" s="6" t="s">
         <v>545</v>
       </c>
+      <c r="E90" t="s">
+        <v>526</v>
+      </c>
       <c r="F90" t="s">
         <v>11</v>
       </c>
@@ -5213,7 +5228,7 @@
         <v>545</v>
       </c>
       <c r="E91" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="F91" t="s">
         <v>11</v>
@@ -5243,9 +5258,6 @@
       </c>
       <c r="D92" s="6" t="s">
         <v>545</v>
-      </c>
-      <c r="E92" t="s">
-        <v>527</v>
       </c>
       <c r="F92" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
New database takeon functionally complete
</commit_message>
<xml_diff>
--- a/db/airr_schema_defs.xlsx
+++ b/db/airr_schema_defs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Research\digby_backend\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9C7A0D9-C8EF-4678-A28D-505D4C994CD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7631EFF-EACF-4F55-A466-A979D6F7C447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="airr_schema_defs" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1099" uniqueCount="655">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1114" uniqueCount="659">
   <si>
     <t>structured_name</t>
   </si>
@@ -1730,9 +1730,6 @@
     <t>Samples</t>
   </si>
   <si>
-    <t>Reads</t>
-  </si>
-  <si>
     <t>Study Ref</t>
   </si>
   <si>
@@ -1761,9 +1758,6 @@
     <t>Sample name as allocated by VDJbase</t>
   </si>
   <si>
-    <t>Number of reads</t>
-  </si>
-  <si>
     <t>Genotype report</t>
   </si>
   <si>
@@ -1890,9 +1884,6 @@
     <t>Germline</t>
   </si>
   <si>
-    <t>Genotype Detections.name</t>
-  </si>
-  <si>
     <t>Genotype Detections.Pre-processing</t>
   </si>
   <si>
@@ -1977,9 +1968,6 @@
     <t>Subjects.Ethnic</t>
   </si>
   <si>
-    <t>Subjects.Sec</t>
-  </si>
-  <si>
     <t>Subjects.Health Status</t>
   </si>
   <si>
@@ -2014,6 +2002,30 @@
   </si>
   <si>
     <t>Aligner ref D</t>
+  </si>
+  <si>
+    <t>Subjects.Sex</t>
+  </si>
+  <si>
+    <t>Samples.Name</t>
+  </si>
+  <si>
+    <t>Subjects.Name</t>
+  </si>
+  <si>
+    <t>Genotype Detections.Name</t>
+  </si>
+  <si>
+    <t>VDJbase reads</t>
+  </si>
+  <si>
+    <t>Reads processed by VDJbase pipeline</t>
+  </si>
+  <si>
+    <t>TRUE if the processed reads are restricted to those that have a single V_call</t>
+  </si>
+  <si>
+    <t>Repertoire or germline</t>
   </si>
 </sst>
 </file>
@@ -2868,8 +2880,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A118" sqref="A118"/>
+    <sheetView tabSelected="1" topLeftCell="F112" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J142" sqref="J142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2901,7 +2913,7 @@
         <v>541</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>3</v>
@@ -3017,7 +3029,7 @@
         <v>515</v>
       </c>
       <c r="F5" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="G5" t="s">
         <v>11</v>
@@ -3220,7 +3232,7 @@
         <v>514</v>
       </c>
       <c r="F12" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="G12" t="s">
         <v>11</v>
@@ -3313,7 +3325,7 @@
         <v>509</v>
       </c>
       <c r="F15" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="G15" t="s">
         <v>11</v>
@@ -3348,7 +3360,7 @@
         <v>510</v>
       </c>
       <c r="F16" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="G16" t="s">
         <v>11</v>
@@ -3383,7 +3395,7 @@
         <v>512</v>
       </c>
       <c r="F17" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="G17" t="s">
         <v>11</v>
@@ -3499,7 +3511,7 @@
         <v>534</v>
       </c>
       <c r="F21" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="G21" t="s">
         <v>11</v>
@@ -3658,7 +3670,7 @@
         <v>529</v>
       </c>
       <c r="F27" t="s">
-        <v>642</v>
+        <v>651</v>
       </c>
       <c r="G27" t="s">
         <v>11</v>
@@ -3832,7 +3844,7 @@
         <v>528</v>
       </c>
       <c r="F33" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
       <c r="G33" t="s">
         <v>11</v>
@@ -3858,7 +3870,7 @@
         <v>535</v>
       </c>
       <c r="F34" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
       <c r="G34" t="s">
         <v>11</v>
@@ -3893,7 +3905,7 @@
         <v>531</v>
       </c>
       <c r="F35" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="G35" t="s">
         <v>11</v>
@@ -4044,7 +4056,7 @@
         <v>533</v>
       </c>
       <c r="F40" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="G40" t="s">
         <v>11</v>
@@ -4105,7 +4117,7 @@
         <v>532</v>
       </c>
       <c r="F42" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="G42" t="s">
         <v>11</v>
@@ -4588,7 +4600,7 @@
         <v>521</v>
       </c>
       <c r="F60" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="G60" t="s">
         <v>11</v>
@@ -4878,7 +4890,7 @@
         <v>517</v>
       </c>
       <c r="F70" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="G70" t="s">
         <v>11</v>
@@ -4910,7 +4922,7 @@
         <v>518</v>
       </c>
       <c r="F71" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="G71" t="s">
         <v>11</v>
@@ -4971,7 +4983,7 @@
         <v>519</v>
       </c>
       <c r="F73" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
       <c r="G73" t="s">
         <v>11</v>
@@ -5203,7 +5215,7 @@
         <v>527</v>
       </c>
       <c r="F81" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="G81" t="s">
         <v>11</v>
@@ -5345,10 +5357,10 @@
         <v>543</v>
       </c>
       <c r="E86" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="F86" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="G86" t="s">
         <v>11</v>
@@ -5441,7 +5453,7 @@
         <v>536</v>
       </c>
       <c r="F89" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="G89" t="s">
         <v>11</v>
@@ -5476,7 +5488,7 @@
         <v>524</v>
       </c>
       <c r="F90" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="G90" t="s">
         <v>11</v>
@@ -5511,7 +5523,7 @@
         <v>525</v>
       </c>
       <c r="F91" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="G91" t="s">
         <v>11</v>
@@ -5598,7 +5610,7 @@
         <v>400</v>
       </c>
       <c r="D94" s="6" t="s">
-        <v>543</v>
+        <v>242</v>
       </c>
       <c r="G94" t="s">
         <v>11</v>
@@ -5627,7 +5639,7 @@
         <v>400</v>
       </c>
       <c r="D95" s="6" t="s">
-        <v>543</v>
+        <v>242</v>
       </c>
       <c r="G95" t="s">
         <v>312</v>
@@ -5662,7 +5674,7 @@
         <v>526</v>
       </c>
       <c r="F96" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="G96" t="s">
         <v>11</v>
@@ -5720,7 +5732,7 @@
         <v>400</v>
       </c>
       <c r="D98" s="6" t="s">
-        <v>543</v>
+        <v>242</v>
       </c>
       <c r="G98" t="s">
         <v>11</v>
@@ -5778,7 +5790,7 @@
         <v>400</v>
       </c>
       <c r="D100" s="6" t="s">
-        <v>543</v>
+        <v>242</v>
       </c>
       <c r="G100" t="s">
         <v>11</v>
@@ -5804,7 +5816,7 @@
         <v>400</v>
       </c>
       <c r="D101" s="6" t="s">
-        <v>543</v>
+        <v>242</v>
       </c>
       <c r="G101" t="s">
         <v>11</v>
@@ -5833,7 +5845,7 @@
         <v>400</v>
       </c>
       <c r="D102" s="6" t="s">
-        <v>543</v>
+        <v>242</v>
       </c>
       <c r="G102" t="s">
         <v>11</v>
@@ -5868,7 +5880,7 @@
         <v>523</v>
       </c>
       <c r="F103" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="G103" t="s">
         <v>312</v>
@@ -5897,7 +5909,7 @@
         <v>400</v>
       </c>
       <c r="D104" s="6" t="s">
-        <v>543</v>
+        <v>242</v>
       </c>
       <c r="G104" t="s">
         <v>11</v>
@@ -5926,7 +5938,7 @@
         <v>400</v>
       </c>
       <c r="D105" s="6" t="s">
-        <v>543</v>
+        <v>242</v>
       </c>
       <c r="G105" t="s">
         <v>11</v>
@@ -6288,7 +6300,7 @@
         <v>546</v>
       </c>
       <c r="F118" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="G118" t="s">
         <v>312</v>
@@ -6317,7 +6329,7 @@
         <v>547</v>
       </c>
       <c r="F119" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="G119" t="s">
         <v>312</v>
@@ -6352,10 +6364,10 @@
         <v>0</v>
       </c>
       <c r="I120" t="s">
+        <v>560</v>
+      </c>
+      <c r="J120" s="1" t="s">
         <v>561</v>
-      </c>
-      <c r="J120" s="1" t="s">
-        <v>562</v>
       </c>
       <c r="L120" t="s">
         <v>513</v>
@@ -6372,7 +6384,7 @@
         <v>549</v>
       </c>
       <c r="F121" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
       <c r="G121" t="s">
         <v>11</v>
@@ -6381,10 +6393,10 @@
         <v>0</v>
       </c>
       <c r="I121" t="s">
+        <v>562</v>
+      </c>
+      <c r="J121" t="s">
         <v>563</v>
-      </c>
-      <c r="J121" t="s">
-        <v>564</v>
       </c>
       <c r="L121" t="s">
         <v>522</v>
@@ -6400,6 +6412,9 @@
       <c r="E122" t="s">
         <v>550</v>
       </c>
+      <c r="F122" t="s">
+        <v>653</v>
+      </c>
       <c r="G122" t="s">
         <v>11</v>
       </c>
@@ -6407,10 +6422,10 @@
         <v>0</v>
       </c>
       <c r="I122" t="s">
+        <v>564</v>
+      </c>
+      <c r="J122" t="s">
         <v>565</v>
-      </c>
-      <c r="J122" t="s">
-        <v>566</v>
       </c>
       <c r="L122" t="s">
         <v>530</v>
@@ -6433,10 +6448,10 @@
         <v>0</v>
       </c>
       <c r="I123" t="s">
+        <v>566</v>
+      </c>
+      <c r="J123" t="s">
         <v>567</v>
-      </c>
-      <c r="J123" t="s">
-        <v>568</v>
       </c>
       <c r="L123" t="s">
         <v>552</v>
@@ -6452,6 +6467,9 @@
       <c r="E124" t="s">
         <v>550</v>
       </c>
+      <c r="F124" t="s">
+        <v>652</v>
+      </c>
       <c r="G124" t="s">
         <v>11</v>
       </c>
@@ -6459,10 +6477,10 @@
         <v>0</v>
       </c>
       <c r="I124" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="J124" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="L124" t="s">
         <v>530</v>
@@ -6479,7 +6497,7 @@
         <v>553</v>
       </c>
       <c r="F125" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="G125" t="s">
         <v>312</v>
@@ -6488,10 +6506,10 @@
         <v>0</v>
       </c>
       <c r="I125" t="s">
-        <v>560</v>
+        <v>655</v>
       </c>
       <c r="J125" t="s">
-        <v>570</v>
+        <v>656</v>
       </c>
       <c r="L125" t="s">
         <v>530</v>
@@ -6514,10 +6532,10 @@
         <v>0</v>
       </c>
       <c r="I126" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="J126" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="L126" t="s">
         <v>511</v>
@@ -6540,10 +6558,10 @@
         <v>0</v>
       </c>
       <c r="I127" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="J127" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="L127" t="s">
         <v>511</v>
@@ -6551,16 +6569,16 @@
     </row>
     <row r="128" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="D128" s="5" t="s">
         <v>242</v>
       </c>
       <c r="E128" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="F128" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="G128" t="s">
         <v>11</v>
@@ -6569,16 +6587,16 @@
         <v>0</v>
       </c>
       <c r="I128" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="J128" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="L128" t="s">
         <v>538</v>
       </c>
     </row>
-    <row r="129" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
         <v>550</v>
       </c>
@@ -6595,24 +6613,24 @@
         <v>0</v>
       </c>
       <c r="I129" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="J129" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="130" spans="2:10" x14ac:dyDescent="0.25">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="130" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
         <v>550</v>
       </c>
       <c r="D130" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="E130" t="s">
         <v>550</v>
       </c>
       <c r="F130" t="s">
-        <v>613</v>
+        <v>654</v>
       </c>
       <c r="G130" t="s">
         <v>11</v>
@@ -6621,24 +6639,27 @@
         <v>0</v>
       </c>
       <c r="I130" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="J130" t="s">
+        <v>608</v>
+      </c>
+      <c r="K130" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="131" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B131" t="s">
+        <v>586</v>
+      </c>
+      <c r="D131" t="s">
+        <v>585</v>
+      </c>
+      <c r="E131" t="s">
+        <v>586</v>
+      </c>
+      <c r="F131" t="s">
         <v>611</v>
-      </c>
-    </row>
-    <row r="131" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B131" t="s">
-        <v>588</v>
-      </c>
-      <c r="D131" t="s">
-        <v>587</v>
-      </c>
-      <c r="E131" t="s">
-        <v>588</v>
-      </c>
-      <c r="F131" t="s">
-        <v>614</v>
       </c>
       <c r="G131" t="s">
         <v>11</v>
@@ -6647,24 +6668,27 @@
         <v>0</v>
       </c>
       <c r="I131" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="J131" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="132" spans="2:10" x14ac:dyDescent="0.25">
+        <v>594</v>
+      </c>
+      <c r="K131" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="132" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="D132" t="s">
+        <v>585</v>
+      </c>
+      <c r="E132" t="s">
         <v>587</v>
       </c>
-      <c r="E132" t="s">
-        <v>589</v>
-      </c>
       <c r="F132" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="G132" t="s">
         <v>11</v>
@@ -6673,24 +6697,27 @@
         <v>0</v>
       </c>
       <c r="I132" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="J132" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="133" spans="2:10" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+      <c r="K132" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="133" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="D133" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="E133" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="F133" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="G133" t="s">
         <v>11</v>
@@ -6699,24 +6726,27 @@
         <v>0</v>
       </c>
       <c r="I133" t="s">
-        <v>599</v>
-      </c>
-      <c r="J133">
+        <v>597</v>
+      </c>
+      <c r="J133" t="s">
+        <v>597</v>
+      </c>
+      <c r="K133">
         <v>1.18</v>
       </c>
     </row>
-    <row r="134" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
+        <v>614</v>
+      </c>
+      <c r="D134" t="s">
+        <v>585</v>
+      </c>
+      <c r="E134" t="s">
+        <v>614</v>
+      </c>
+      <c r="F134" t="s">
         <v>617</v>
-      </c>
-      <c r="D134" t="s">
-        <v>587</v>
-      </c>
-      <c r="E134" t="s">
-        <v>617</v>
-      </c>
-      <c r="F134" t="s">
-        <v>620</v>
       </c>
       <c r="G134" t="s">
         <v>11</v>
@@ -6725,24 +6755,27 @@
         <v>0</v>
       </c>
       <c r="I134" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="J134" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="135" spans="2:10" x14ac:dyDescent="0.25">
+        <v>649</v>
+      </c>
+      <c r="K134" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="135" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
+        <v>615</v>
+      </c>
+      <c r="D135" t="s">
+        <v>585</v>
+      </c>
+      <c r="E135" t="s">
+        <v>615</v>
+      </c>
+      <c r="F135" t="s">
         <v>618</v>
-      </c>
-      <c r="D135" t="s">
-        <v>587</v>
-      </c>
-      <c r="E135" t="s">
-        <v>618</v>
-      </c>
-      <c r="F135" t="s">
-        <v>621</v>
       </c>
       <c r="G135" t="s">
         <v>11</v>
@@ -6751,24 +6784,27 @@
         <v>0</v>
       </c>
       <c r="I135" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="J135" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="136" spans="2:10" x14ac:dyDescent="0.25">
+        <v>650</v>
+      </c>
+      <c r="K135" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="136" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B136" t="s">
+        <v>616</v>
+      </c>
+      <c r="D136" t="s">
+        <v>585</v>
+      </c>
+      <c r="E136" t="s">
+        <v>616</v>
+      </c>
+      <c r="F136" t="s">
         <v>619</v>
-      </c>
-      <c r="D136" t="s">
-        <v>587</v>
-      </c>
-      <c r="E136" t="s">
-        <v>619</v>
-      </c>
-      <c r="F136" t="s">
-        <v>622</v>
       </c>
       <c r="G136" t="s">
         <v>11</v>
@@ -6777,24 +6813,27 @@
         <v>0</v>
       </c>
       <c r="I136" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
       <c r="J136" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="137" spans="2:10" x14ac:dyDescent="0.25">
+        <v>647</v>
+      </c>
+      <c r="K136" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="137" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="D137" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="E137" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="F137" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="G137" t="s">
         <v>11</v>
@@ -6803,24 +6842,27 @@
         <v>0</v>
       </c>
       <c r="I137" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="J137" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="138" spans="2:10" x14ac:dyDescent="0.25">
+        <v>598</v>
+      </c>
+      <c r="K137" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="138" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B138" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="D138" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="E138" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="F138" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="G138" t="s">
         <v>11</v>
@@ -6829,24 +6871,27 @@
         <v>0</v>
       </c>
       <c r="I138" t="s">
-        <v>601</v>
-      </c>
-      <c r="J138">
+        <v>599</v>
+      </c>
+      <c r="J138" t="s">
+        <v>599</v>
+      </c>
+      <c r="K138">
         <v>1.2</v>
       </c>
     </row>
-    <row r="139" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B139" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="D139" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="E139" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="F139" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="G139" t="s">
         <v>11</v>
@@ -6855,24 +6900,27 @@
         <v>0</v>
       </c>
       <c r="I139" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="J139" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="140" spans="2:10" x14ac:dyDescent="0.25">
+        <v>600</v>
+      </c>
+      <c r="K139" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="140" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="D140" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="E140" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="F140" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="G140" t="s">
         <v>11</v>
@@ -6881,24 +6929,27 @@
         <v>0</v>
       </c>
       <c r="I140" t="s">
-        <v>603</v>
-      </c>
-      <c r="J140">
+        <v>601</v>
+      </c>
+      <c r="J140" t="s">
+        <v>601</v>
+      </c>
+      <c r="K140">
         <v>1.2</v>
       </c>
     </row>
-    <row r="141" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="D141" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="E141" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="F141" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="G141" t="s">
         <v>104</v>
@@ -6907,24 +6958,27 @@
         <v>0</v>
       </c>
       <c r="I141" t="s">
-        <v>598</v>
-      </c>
-      <c r="J141" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="142" spans="2:10" x14ac:dyDescent="0.25">
+        <v>596</v>
+      </c>
+      <c r="J141" t="s">
+        <v>657</v>
+      </c>
+      <c r="K141" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B142" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="D142" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="E142" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="F142" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="G142" t="s">
         <v>11</v>
@@ -6933,10 +6987,13 @@
         <v>0</v>
       </c>
       <c r="I142" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="J142" t="s">
-        <v>612</v>
+        <v>658</v>
+      </c>
+      <c r="K142" t="s">
+        <v>610</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Column defs and fixes
</commit_message>
<xml_diff>
--- a/db/airr_schema_defs.xlsx
+++ b/db/airr_schema_defs.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Research\digby_backend\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7849D87B-A0E6-46E2-B61E-627ABA74717C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64A0E5F8-B7C9-4B72-8B4D-168BF1886502}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="airr_schema_defs" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">airr_schema_defs!$A$1:$L$143</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">airr_schema_defs!$A$1:$O$143</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1117" uniqueCount="664">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1265" uniqueCount="672">
   <si>
     <t>structured_name</t>
   </si>
@@ -2044,6 +2044,30 @@
   </si>
   <si>
     <t>sample_name</t>
+  </si>
+  <si>
+    <t>display</t>
+  </si>
+  <si>
+    <t>hide</t>
+  </si>
+  <si>
+    <t>size</t>
+  </si>
+  <si>
+    <t>short</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
+    <t>Organism ID</t>
+  </si>
+  <si>
+    <t>Organism label</t>
+  </si>
+  <si>
+    <t>Age</t>
   </si>
 </sst>
 </file>
@@ -2896,10 +2920,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L143"/>
+  <dimension ref="A1:O143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B127" sqref="B127"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H49" sqref="H49:H54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2909,12 +2933,12 @@
     <col min="3" max="4" width="27.140625" customWidth="1"/>
     <col min="5" max="5" width="28" customWidth="1"/>
     <col min="6" max="6" width="39.28515625" customWidth="1"/>
-    <col min="9" max="9" width="35.42578125" customWidth="1"/>
-    <col min="10" max="10" width="148.28515625" customWidth="1"/>
-    <col min="11" max="11" width="58.42578125" customWidth="1"/>
+    <col min="12" max="12" width="35.42578125" customWidth="1"/>
+    <col min="13" max="13" width="148.28515625" customWidth="1"/>
+    <col min="14" max="14" width="58.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2937,22 +2961,31 @@
         <v>3</v>
       </c>
       <c r="H1" s="3" t="s">
+        <v>664</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>665</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>666</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>544</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -2969,16 +3002,25 @@
         <v>11</v>
       </c>
       <c r="H2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>667</v>
+      </c>
+      <c r="K2" t="b">
         <v>0</v>
       </c>
-      <c r="I2" t="s">
+      <c r="L2" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -2995,16 +3037,25 @@
         <v>11</v>
       </c>
       <c r="H3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
+        <v>668</v>
+      </c>
+      <c r="K3" t="b">
         <v>0</v>
       </c>
-      <c r="I3" t="s">
+      <c r="L3" t="s">
         <v>16</v>
       </c>
-      <c r="J3" t="s">
+      <c r="M3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -3021,16 +3072,25 @@
         <v>11</v>
       </c>
       <c r="H4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J4" t="s">
+        <v>668</v>
+      </c>
+      <c r="K4" t="b">
         <v>0</v>
       </c>
-      <c r="I4" t="s">
+      <c r="L4" t="s">
         <v>20</v>
       </c>
-      <c r="J4" t="s">
+      <c r="M4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -3053,19 +3113,28 @@
         <v>11</v>
       </c>
       <c r="H5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J5" t="s">
+        <v>667</v>
+      </c>
+      <c r="K5" t="b">
         <v>0</v>
       </c>
-      <c r="I5" t="s">
+      <c r="L5" t="s">
         <v>25</v>
       </c>
-      <c r="J5" t="s">
+      <c r="M5" t="s">
         <v>26</v>
       </c>
-      <c r="K5" t="s">
+      <c r="N5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -3082,19 +3151,28 @@
         <v>11</v>
       </c>
       <c r="H6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J6" t="s">
+        <v>668</v>
+      </c>
+      <c r="K6" t="b">
         <v>0</v>
       </c>
-      <c r="I6" t="s">
+      <c r="L6" t="s">
         <v>30</v>
       </c>
-      <c r="J6" t="s">
+      <c r="M6" t="s">
         <v>31</v>
       </c>
-      <c r="K6" t="s">
+      <c r="N6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -3111,16 +3189,25 @@
         <v>11</v>
       </c>
       <c r="H7" t="b">
+        <v>1</v>
+      </c>
+      <c r="I7" t="b">
+        <v>1</v>
+      </c>
+      <c r="J7" t="s">
+        <v>668</v>
+      </c>
+      <c r="K7" t="b">
         <v>0</v>
       </c>
-      <c r="I7" t="s">
+      <c r="L7" t="s">
         <v>35</v>
       </c>
-      <c r="J7" t="s">
+      <c r="M7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -3137,16 +3224,25 @@
         <v>11</v>
       </c>
       <c r="H8" t="b">
+        <v>1</v>
+      </c>
+      <c r="I8" t="b">
+        <v>1</v>
+      </c>
+      <c r="J8" t="s">
+        <v>668</v>
+      </c>
+      <c r="K8" t="b">
         <v>0</v>
       </c>
-      <c r="I8" t="s">
+      <c r="L8" t="s">
         <v>35</v>
       </c>
-      <c r="J8" t="s">
+      <c r="M8" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -3163,19 +3259,28 @@
         <v>11</v>
       </c>
       <c r="H9" t="b">
+        <v>1</v>
+      </c>
+      <c r="I9" t="b">
+        <v>1</v>
+      </c>
+      <c r="J9" t="s">
+        <v>668</v>
+      </c>
+      <c r="K9" t="b">
         <v>0</v>
       </c>
-      <c r="I9" t="s">
+      <c r="L9" t="s">
         <v>42</v>
       </c>
-      <c r="J9" t="s">
+      <c r="M9" t="s">
         <v>43</v>
       </c>
-      <c r="K9" t="s">
+      <c r="N9" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -3192,19 +3297,28 @@
         <v>11</v>
       </c>
       <c r="H10" t="b">
+        <v>1</v>
+      </c>
+      <c r="I10" t="b">
+        <v>1</v>
+      </c>
+      <c r="J10" t="s">
+        <v>668</v>
+      </c>
+      <c r="K10" t="b">
         <v>0</v>
       </c>
-      <c r="I10" t="s">
+      <c r="L10" t="s">
         <v>47</v>
       </c>
-      <c r="J10" t="s">
+      <c r="M10" t="s">
         <v>48</v>
       </c>
-      <c r="K10" t="s">
+      <c r="N10" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>50</v>
       </c>
@@ -3221,19 +3335,28 @@
         <v>11</v>
       </c>
       <c r="H11" t="b">
+        <v>1</v>
+      </c>
+      <c r="I11" t="b">
+        <v>1</v>
+      </c>
+      <c r="J11" t="s">
+        <v>668</v>
+      </c>
+      <c r="K11" t="b">
         <v>0</v>
       </c>
-      <c r="I11" t="s">
+      <c r="L11" t="s">
         <v>52</v>
       </c>
-      <c r="J11" t="s">
+      <c r="M11" t="s">
         <v>53</v>
       </c>
-      <c r="K11" t="s">
+      <c r="N11" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>55</v>
       </c>
@@ -3256,19 +3379,28 @@
         <v>11</v>
       </c>
       <c r="H12" t="b">
+        <v>1</v>
+      </c>
+      <c r="I12" t="b">
+        <v>1</v>
+      </c>
+      <c r="J12" t="s">
+        <v>668</v>
+      </c>
+      <c r="K12" t="b">
         <v>0</v>
       </c>
-      <c r="I12" t="s">
+      <c r="L12" t="s">
         <v>57</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="M12" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="K12" t="s">
+      <c r="N12" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -3285,19 +3417,28 @@
         <v>11</v>
       </c>
       <c r="H13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I13" t="b">
+        <v>1</v>
+      </c>
+      <c r="J13" t="s">
+        <v>668</v>
+      </c>
+      <c r="K13" t="b">
         <v>0</v>
       </c>
-      <c r="I13" t="s">
+      <c r="L13" t="s">
         <v>62</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="M13" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="K13" t="s">
+      <c r="N13" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>65</v>
       </c>
@@ -3314,19 +3455,28 @@
         <v>11</v>
       </c>
       <c r="H14" t="b">
+        <v>1</v>
+      </c>
+      <c r="I14" t="b">
+        <v>1</v>
+      </c>
+      <c r="J14" t="s">
+        <v>668</v>
+      </c>
+      <c r="K14" t="b">
         <v>0</v>
       </c>
-      <c r="I14" t="s">
+      <c r="L14" t="s">
         <v>67</v>
       </c>
-      <c r="J14" t="s">
+      <c r="M14" t="s">
         <v>68</v>
       </c>
-      <c r="K14" t="s">
+      <c r="N14" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>70</v>
       </c>
@@ -3349,19 +3499,28 @@
         <v>11</v>
       </c>
       <c r="H15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I15" t="b">
+        <v>1</v>
+      </c>
+      <c r="J15" t="s">
+        <v>668</v>
+      </c>
+      <c r="K15" t="b">
         <v>0</v>
       </c>
-      <c r="I15" t="s">
+      <c r="L15" t="s">
         <v>72</v>
       </c>
-      <c r="J15" t="s">
+      <c r="M15" t="s">
         <v>73</v>
       </c>
-      <c r="K15" t="s">
+      <c r="N15" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>75</v>
       </c>
@@ -3384,19 +3543,28 @@
         <v>11</v>
       </c>
       <c r="H16" t="b">
+        <v>1</v>
+      </c>
+      <c r="I16" t="b">
+        <v>1</v>
+      </c>
+      <c r="J16" t="s">
+        <v>668</v>
+      </c>
+      <c r="K16" t="b">
         <v>0</v>
       </c>
-      <c r="I16" t="s">
+      <c r="L16" t="s">
         <v>77</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="M16" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="K16" t="s">
+      <c r="N16" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>80</v>
       </c>
@@ -3419,19 +3587,28 @@
         <v>11</v>
       </c>
       <c r="H17" t="b">
+        <v>1</v>
+      </c>
+      <c r="I17" t="b">
+        <v>1</v>
+      </c>
+      <c r="J17" t="s">
+        <v>668</v>
+      </c>
+      <c r="K17" t="b">
         <v>0</v>
       </c>
-      <c r="I17" t="s">
+      <c r="L17" t="s">
         <v>82</v>
       </c>
-      <c r="J17" t="s">
+      <c r="M17" t="s">
         <v>83</v>
       </c>
-      <c r="K17" t="s">
+      <c r="N17" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>85</v>
       </c>
@@ -3450,11 +3627,20 @@
       <c r="H18" t="b">
         <v>1</v>
       </c>
-      <c r="I18" t="s">
+      <c r="I18" t="b">
+        <v>1</v>
+      </c>
+      <c r="J18" t="s">
+        <v>668</v>
+      </c>
+      <c r="K18" t="b">
+        <v>1</v>
+      </c>
+      <c r="L18" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>88</v>
       </c>
@@ -3471,19 +3657,28 @@
         <v>11</v>
       </c>
       <c r="H19" t="b">
+        <v>1</v>
+      </c>
+      <c r="I19" t="b">
+        <v>1</v>
+      </c>
+      <c r="J19" t="s">
+        <v>668</v>
+      </c>
+      <c r="K19" t="b">
         <v>0</v>
       </c>
-      <c r="I19" t="s">
+      <c r="L19" t="s">
         <v>90</v>
       </c>
-      <c r="J19" s="1" t="s">
+      <c r="M19" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="K19" s="2">
+      <c r="N19" s="2">
         <v>44229</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>92</v>
       </c>
@@ -3500,19 +3695,28 @@
         <v>11</v>
       </c>
       <c r="H20" t="b">
+        <v>1</v>
+      </c>
+      <c r="I20" t="b">
+        <v>1</v>
+      </c>
+      <c r="J20" t="s">
+        <v>668</v>
+      </c>
+      <c r="K20" t="b">
         <v>0</v>
       </c>
-      <c r="I20" t="s">
+      <c r="L20" t="s">
         <v>94</v>
       </c>
-      <c r="J20" s="1" t="s">
+      <c r="M20" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="K20" s="2">
+      <c r="N20" s="2">
         <v>44229</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>96</v>
       </c>
@@ -3535,19 +3739,28 @@
         <v>11</v>
       </c>
       <c r="H21" t="b">
+        <v>1</v>
+      </c>
+      <c r="I21" t="b">
+        <v>1</v>
+      </c>
+      <c r="J21" t="s">
+        <v>667</v>
+      </c>
+      <c r="K21" t="b">
         <v>0</v>
       </c>
-      <c r="I21" t="s">
+      <c r="L21" t="s">
         <v>99</v>
       </c>
-      <c r="J21" t="s">
+      <c r="M21" t="s">
         <v>100</v>
       </c>
-      <c r="K21" t="s">
+      <c r="N21" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>102</v>
       </c>
@@ -3564,16 +3777,25 @@
         <v>104</v>
       </c>
       <c r="H22" t="b">
+        <v>1</v>
+      </c>
+      <c r="I22" t="b">
+        <v>1</v>
+      </c>
+      <c r="J22" t="s">
+        <v>668</v>
+      </c>
+      <c r="K22" t="b">
         <v>0</v>
       </c>
-      <c r="I22" t="s">
+      <c r="L22" t="s">
         <v>105</v>
       </c>
-      <c r="J22" t="s">
+      <c r="M22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>107</v>
       </c>
@@ -3590,16 +3812,25 @@
         <v>11</v>
       </c>
       <c r="H23" t="b">
+        <v>1</v>
+      </c>
+      <c r="I23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J23" t="s">
+        <v>668</v>
+      </c>
+      <c r="K23" t="b">
         <v>0</v>
       </c>
-      <c r="I23" t="s">
+      <c r="L23" t="s">
         <v>109</v>
       </c>
-      <c r="J23" t="s">
+      <c r="M23" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>110</v>
       </c>
@@ -3616,16 +3847,25 @@
         <v>11</v>
       </c>
       <c r="H24" t="b">
+        <v>1</v>
+      </c>
+      <c r="I24" t="b">
+        <v>1</v>
+      </c>
+      <c r="J24" t="s">
+        <v>667</v>
+      </c>
+      <c r="K24" t="b">
         <v>0</v>
       </c>
-      <c r="I24" t="s">
+      <c r="L24" t="s">
         <v>109</v>
       </c>
-      <c r="J24" t="s">
+      <c r="M24" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>112</v>
       </c>
@@ -3642,13 +3882,25 @@
         <v>11</v>
       </c>
       <c r="H25" t="b">
+        <v>1</v>
+      </c>
+      <c r="I25" t="b">
+        <v>1</v>
+      </c>
+      <c r="J25" t="s">
+        <v>668</v>
+      </c>
+      <c r="K25" t="b">
         <v>0</v>
       </c>
-      <c r="J25" t="s">
+      <c r="L25" t="s">
+        <v>669</v>
+      </c>
+      <c r="M25" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>114</v>
       </c>
@@ -3665,13 +3917,25 @@
         <v>11</v>
       </c>
       <c r="H26" t="b">
+        <v>1</v>
+      </c>
+      <c r="I26" t="b">
+        <v>1</v>
+      </c>
+      <c r="J26" t="s">
+        <v>668</v>
+      </c>
+      <c r="K26" t="b">
         <v>0</v>
       </c>
-      <c r="J26" t="s">
+      <c r="L26" t="s">
+        <v>670</v>
+      </c>
+      <c r="M26" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>116</v>
       </c>
@@ -3694,19 +3958,28 @@
         <v>11</v>
       </c>
       <c r="H27" t="b">
+        <v>1</v>
+      </c>
+      <c r="I27" t="b">
+        <v>1</v>
+      </c>
+      <c r="J27" t="s">
+        <v>667</v>
+      </c>
+      <c r="K27" t="b">
         <v>0</v>
       </c>
-      <c r="I27" t="s">
+      <c r="L27" t="s">
         <v>118</v>
       </c>
-      <c r="J27" t="s">
+      <c r="M27" t="s">
         <v>119</v>
       </c>
-      <c r="K27" t="s">
+      <c r="N27" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>121</v>
       </c>
@@ -3723,19 +3996,28 @@
         <v>660</v>
       </c>
       <c r="H28" t="b">
+        <v>1</v>
+      </c>
+      <c r="I28" t="b">
+        <v>1</v>
+      </c>
+      <c r="J28" t="s">
+        <v>667</v>
+      </c>
+      <c r="K28" t="b">
         <v>0</v>
       </c>
-      <c r="I28" t="s">
+      <c r="L28" t="s">
         <v>123</v>
       </c>
-      <c r="J28" t="s">
+      <c r="M28" t="s">
         <v>124</v>
       </c>
-      <c r="K28">
+      <c r="N28">
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>125</v>
       </c>
@@ -3752,19 +4034,28 @@
         <v>660</v>
       </c>
       <c r="H29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I29" t="b">
+        <v>1</v>
+      </c>
+      <c r="J29" t="s">
+        <v>667</v>
+      </c>
+      <c r="K29" t="b">
         <v>0</v>
       </c>
-      <c r="I29" t="s">
+      <c r="L29" t="s">
         <v>127</v>
       </c>
-      <c r="J29" s="1" t="s">
+      <c r="M29" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="K29">
+      <c r="N29">
         <v>80</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>129</v>
       </c>
@@ -3781,16 +4072,25 @@
         <v>11</v>
       </c>
       <c r="H30" t="b">
+        <v>1</v>
+      </c>
+      <c r="I30" t="b">
+        <v>1</v>
+      </c>
+      <c r="J30" t="s">
+        <v>667</v>
+      </c>
+      <c r="K30" t="b">
         <v>0</v>
       </c>
-      <c r="I30" t="s">
+      <c r="L30" t="s">
         <v>131</v>
       </c>
-      <c r="J30" t="s">
+      <c r="M30" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>132</v>
       </c>
@@ -3807,16 +4107,25 @@
         <v>11</v>
       </c>
       <c r="H31" t="b">
+        <v>1</v>
+      </c>
+      <c r="I31" t="b">
+        <v>1</v>
+      </c>
+      <c r="J31" t="s">
+        <v>667</v>
+      </c>
+      <c r="K31" t="b">
         <v>0</v>
       </c>
-      <c r="I31" t="s">
+      <c r="L31" t="s">
         <v>131</v>
       </c>
-      <c r="J31" t="s">
+      <c r="M31" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>134</v>
       </c>
@@ -3833,19 +4142,28 @@
         <v>11</v>
       </c>
       <c r="H32" t="b">
+        <v>1</v>
+      </c>
+      <c r="I32" t="b">
+        <v>1</v>
+      </c>
+      <c r="J32" t="s">
+        <v>668</v>
+      </c>
+      <c r="K32" t="b">
         <v>0</v>
       </c>
-      <c r="I32" t="s">
+      <c r="L32" t="s">
         <v>136</v>
       </c>
-      <c r="J32" s="1" t="s">
+      <c r="M32" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="K32" t="s">
+      <c r="N32" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>139</v>
       </c>
@@ -3868,10 +4186,22 @@
         <v>11</v>
       </c>
       <c r="H33" t="b">
+        <v>1</v>
+      </c>
+      <c r="I33" t="b">
+        <v>1</v>
+      </c>
+      <c r="J33" t="s">
+        <v>667</v>
+      </c>
+      <c r="K33" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L33" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>141</v>
       </c>
@@ -3894,19 +4224,28 @@
         <v>11</v>
       </c>
       <c r="H34" t="b">
+        <v>1</v>
+      </c>
+      <c r="I34" t="b">
+        <v>1</v>
+      </c>
+      <c r="J34" t="s">
+        <v>667</v>
+      </c>
+      <c r="K34" t="b">
         <v>0</v>
       </c>
-      <c r="I34" t="s">
+      <c r="L34" t="s">
         <v>143</v>
       </c>
-      <c r="J34" t="s">
+      <c r="M34" t="s">
         <v>144</v>
       </c>
-      <c r="K34" t="s">
+      <c r="N34" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>146</v>
       </c>
@@ -3929,19 +4268,28 @@
         <v>11</v>
       </c>
       <c r="H35" t="b">
+        <v>1</v>
+      </c>
+      <c r="I35" t="b">
+        <v>1</v>
+      </c>
+      <c r="J35" t="s">
+        <v>667</v>
+      </c>
+      <c r="K35" t="b">
         <v>0</v>
       </c>
-      <c r="I35" t="s">
+      <c r="L35" t="s">
         <v>148</v>
       </c>
-      <c r="J35" t="s">
+      <c r="M35" t="s">
         <v>149</v>
       </c>
-      <c r="K35" t="s">
+      <c r="N35" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>151</v>
       </c>
@@ -3958,19 +4306,28 @@
         <v>11</v>
       </c>
       <c r="H36" t="b">
+        <v>1</v>
+      </c>
+      <c r="I36" t="b">
+        <v>1</v>
+      </c>
+      <c r="J36" t="s">
+        <v>667</v>
+      </c>
+      <c r="K36" t="b">
         <v>0</v>
       </c>
-      <c r="I36" t="s">
+      <c r="L36" t="s">
         <v>153</v>
       </c>
-      <c r="J36" t="s">
+      <c r="M36" t="s">
         <v>154</v>
       </c>
-      <c r="K36" t="s">
+      <c r="N36" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>156</v>
       </c>
@@ -3987,19 +4344,28 @@
         <v>11</v>
       </c>
       <c r="H37" t="b">
+        <v>1</v>
+      </c>
+      <c r="I37" t="b">
+        <v>1</v>
+      </c>
+      <c r="J37" t="s">
+        <v>668</v>
+      </c>
+      <c r="K37" t="b">
         <v>0</v>
       </c>
-      <c r="I37" t="s">
+      <c r="L37" t="s">
         <v>158</v>
       </c>
-      <c r="J37" t="s">
+      <c r="M37" t="s">
         <v>159</v>
       </c>
-      <c r="K37" t="s">
+      <c r="N37" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>161</v>
       </c>
@@ -4016,19 +4382,28 @@
         <v>11</v>
       </c>
       <c r="H38" t="b">
+        <v>1</v>
+      </c>
+      <c r="I38" t="b">
+        <v>1</v>
+      </c>
+      <c r="J38" t="s">
+        <v>668</v>
+      </c>
+      <c r="K38" t="b">
         <v>0</v>
       </c>
-      <c r="I38" t="s">
+      <c r="L38" t="s">
         <v>163</v>
       </c>
-      <c r="J38" t="s">
+      <c r="M38" t="s">
         <v>164</v>
       </c>
-      <c r="K38" t="s">
+      <c r="N38" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>166</v>
       </c>
@@ -4045,19 +4420,28 @@
         <v>11</v>
       </c>
       <c r="H39" t="b">
+        <v>1</v>
+      </c>
+      <c r="I39" t="b">
+        <v>1</v>
+      </c>
+      <c r="J39" t="s">
+        <v>668</v>
+      </c>
+      <c r="K39" t="b">
         <v>0</v>
       </c>
-      <c r="I39" t="s">
+      <c r="L39" t="s">
         <v>168</v>
       </c>
-      <c r="J39" t="s">
+      <c r="M39" t="s">
         <v>169</v>
       </c>
-      <c r="K39" t="s">
+      <c r="N39" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>171</v>
       </c>
@@ -4082,17 +4466,26 @@
       <c r="H40" t="b">
         <v>1</v>
       </c>
-      <c r="I40" t="s">
+      <c r="I40" t="b">
+        <v>1</v>
+      </c>
+      <c r="J40" t="s">
+        <v>668</v>
+      </c>
+      <c r="K40" t="b">
+        <v>1</v>
+      </c>
+      <c r="L40" t="s">
         <v>173</v>
       </c>
-      <c r="J40" t="s">
+      <c r="M40" t="s">
         <v>174</v>
       </c>
-      <c r="K40" t="s">
+      <c r="N40" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>176</v>
       </c>
@@ -4111,14 +4504,23 @@
       <c r="H41" t="b">
         <v>1</v>
       </c>
-      <c r="I41" t="s">
+      <c r="I41" t="b">
+        <v>1</v>
+      </c>
+      <c r="J41" t="s">
+        <v>668</v>
+      </c>
+      <c r="K41" t="b">
+        <v>1</v>
+      </c>
+      <c r="L41" t="s">
         <v>178</v>
       </c>
-      <c r="J41" t="s">
+      <c r="M41" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>179</v>
       </c>
@@ -4143,14 +4545,23 @@
       <c r="H42" t="b">
         <v>1</v>
       </c>
-      <c r="I42" t="s">
+      <c r="I42" t="b">
+        <v>1</v>
+      </c>
+      <c r="J42" t="s">
+        <v>668</v>
+      </c>
+      <c r="K42" t="b">
+        <v>1</v>
+      </c>
+      <c r="L42" t="s">
         <v>178</v>
       </c>
-      <c r="J42" t="s">
+      <c r="M42" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>181</v>
       </c>
@@ -4169,17 +4580,26 @@
       <c r="H43" t="b">
         <v>1</v>
       </c>
-      <c r="I43" t="s">
+      <c r="I43" t="b">
+        <v>1</v>
+      </c>
+      <c r="J43" t="s">
+        <v>668</v>
+      </c>
+      <c r="K43" t="b">
+        <v>1</v>
+      </c>
+      <c r="L43" t="s">
         <v>183</v>
       </c>
-      <c r="J43" t="s">
+      <c r="M43" t="s">
         <v>184</v>
       </c>
-      <c r="K43" t="s">
+      <c r="N43" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>186</v>
       </c>
@@ -4198,17 +4618,26 @@
       <c r="H44" t="b">
         <v>1</v>
       </c>
-      <c r="I44" t="s">
+      <c r="I44" t="b">
+        <v>1</v>
+      </c>
+      <c r="J44" t="s">
+        <v>668</v>
+      </c>
+      <c r="K44" t="b">
+        <v>1</v>
+      </c>
+      <c r="L44" t="s">
         <v>188</v>
       </c>
-      <c r="J44" t="s">
+      <c r="M44" t="s">
         <v>189</v>
       </c>
-      <c r="K44" t="s">
+      <c r="N44" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>191</v>
       </c>
@@ -4227,17 +4656,26 @@
       <c r="H45" t="b">
         <v>1</v>
       </c>
-      <c r="I45" t="s">
+      <c r="I45" t="b">
+        <v>1</v>
+      </c>
+      <c r="J45" t="s">
+        <v>668</v>
+      </c>
+      <c r="K45" t="b">
+        <v>1</v>
+      </c>
+      <c r="L45" t="s">
         <v>193</v>
       </c>
-      <c r="J45" t="s">
+      <c r="M45" t="s">
         <v>194</v>
       </c>
-      <c r="K45" t="s">
+      <c r="N45" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>196</v>
       </c>
@@ -4256,17 +4694,26 @@
       <c r="H46" t="b">
         <v>1</v>
       </c>
-      <c r="I46" t="s">
+      <c r="I46" t="b">
+        <v>1</v>
+      </c>
+      <c r="J46" t="s">
+        <v>668</v>
+      </c>
+      <c r="K46" t="b">
+        <v>1</v>
+      </c>
+      <c r="L46" t="s">
         <v>198</v>
       </c>
-      <c r="J46" t="s">
+      <c r="M46" t="s">
         <v>199</v>
       </c>
-      <c r="K46" t="s">
+      <c r="N46" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>201</v>
       </c>
@@ -4285,17 +4732,26 @@
       <c r="H47" t="b">
         <v>1</v>
       </c>
-      <c r="I47" t="s">
+      <c r="I47" t="b">
+        <v>1</v>
+      </c>
+      <c r="J47" t="s">
+        <v>668</v>
+      </c>
+      <c r="K47" t="b">
+        <v>1</v>
+      </c>
+      <c r="L47" t="s">
         <v>203</v>
       </c>
-      <c r="J47" t="s">
+      <c r="M47" t="s">
         <v>204</v>
       </c>
-      <c r="K47" t="s">
+      <c r="N47" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>206</v>
       </c>
@@ -4314,17 +4770,26 @@
       <c r="H48" t="b">
         <v>1</v>
       </c>
-      <c r="I48" t="s">
+      <c r="I48" t="b">
+        <v>1</v>
+      </c>
+      <c r="J48" t="s">
+        <v>668</v>
+      </c>
+      <c r="K48" t="b">
+        <v>1</v>
+      </c>
+      <c r="L48" t="s">
         <v>208</v>
       </c>
-      <c r="J48" t="s">
+      <c r="M48" t="s">
         <v>209</v>
       </c>
-      <c r="K48" t="s">
+      <c r="N48" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>211</v>
       </c>
@@ -4343,11 +4808,20 @@
       <c r="H49" t="b">
         <v>0</v>
       </c>
+      <c r="I49" t="b">
+        <v>1</v>
+      </c>
       <c r="J49" t="s">
+        <v>668</v>
+      </c>
+      <c r="K49" t="b">
+        <v>0</v>
+      </c>
+      <c r="M49" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>214</v>
       </c>
@@ -4366,11 +4840,20 @@
       <c r="H50" t="b">
         <v>0</v>
       </c>
+      <c r="I50" t="b">
+        <v>1</v>
+      </c>
       <c r="J50" t="s">
+        <v>668</v>
+      </c>
+      <c r="K50" t="b">
+        <v>0</v>
+      </c>
+      <c r="M50" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>217</v>
       </c>
@@ -4387,13 +4870,22 @@
         <v>11</v>
       </c>
       <c r="H51" t="b">
+        <v>0</v>
+      </c>
+      <c r="I51" t="b">
         <v>1</v>
       </c>
       <c r="J51" t="s">
+        <v>668</v>
+      </c>
+      <c r="K51" t="b">
+        <v>1</v>
+      </c>
+      <c r="M51" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>220</v>
       </c>
@@ -4410,13 +4902,22 @@
         <v>11</v>
       </c>
       <c r="H52" t="b">
-        <v>1</v>
-      </c>
-      <c r="K52" t="s">
+        <v>0</v>
+      </c>
+      <c r="I52" t="b">
+        <v>1</v>
+      </c>
+      <c r="J52" t="s">
+        <v>668</v>
+      </c>
+      <c r="K52" t="b">
+        <v>1</v>
+      </c>
+      <c r="N52" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>223</v>
       </c>
@@ -4433,13 +4934,22 @@
         <v>11</v>
       </c>
       <c r="H53" t="b">
+        <v>0</v>
+      </c>
+      <c r="I53" t="b">
         <v>1</v>
       </c>
       <c r="J53" t="s">
+        <v>668</v>
+      </c>
+      <c r="K53" t="b">
+        <v>1</v>
+      </c>
+      <c r="M53" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>226</v>
       </c>
@@ -4456,13 +4966,22 @@
         <v>11</v>
       </c>
       <c r="H54" t="b">
+        <v>0</v>
+      </c>
+      <c r="I54" t="b">
         <v>1</v>
       </c>
       <c r="J54" t="s">
+        <v>668</v>
+      </c>
+      <c r="K54" t="b">
+        <v>1</v>
+      </c>
+      <c r="M54" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>229</v>
       </c>
@@ -4481,17 +5000,26 @@
       <c r="H55" t="b">
         <v>1</v>
       </c>
-      <c r="I55" t="s">
+      <c r="I55" t="b">
+        <v>1</v>
+      </c>
+      <c r="J55" t="s">
+        <v>668</v>
+      </c>
+      <c r="K55" t="b">
+        <v>1</v>
+      </c>
+      <c r="L55" t="s">
         <v>231</v>
       </c>
-      <c r="J55" t="s">
+      <c r="M55" t="s">
         <v>232</v>
       </c>
-      <c r="K55" t="s">
+      <c r="N55" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>234</v>
       </c>
@@ -4510,14 +5038,23 @@
       <c r="H56" t="b">
         <v>1</v>
       </c>
-      <c r="I56" t="s">
+      <c r="I56" t="b">
+        <v>1</v>
+      </c>
+      <c r="J56" t="s">
+        <v>668</v>
+      </c>
+      <c r="K56" t="b">
+        <v>1</v>
+      </c>
+      <c r="L56" t="s">
         <v>237</v>
       </c>
-      <c r="J56" s="1" t="s">
+      <c r="M56" s="1" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>239</v>
       </c>
@@ -4536,17 +5073,26 @@
       <c r="H57" t="b">
         <v>1</v>
       </c>
-      <c r="I57" t="s">
+      <c r="I57" t="b">
+        <v>1</v>
+      </c>
+      <c r="J57" t="s">
+        <v>668</v>
+      </c>
+      <c r="K57" t="b">
+        <v>1</v>
+      </c>
+      <c r="L57" t="s">
         <v>242</v>
       </c>
-      <c r="J57" t="s">
+      <c r="M57" t="s">
         <v>243</v>
       </c>
-      <c r="K57" t="s">
+      <c r="N57" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>245</v>
       </c>
@@ -4565,17 +5111,26 @@
       <c r="H58" t="b">
         <v>1</v>
       </c>
-      <c r="I58" t="s">
+      <c r="I58" t="b">
+        <v>1</v>
+      </c>
+      <c r="J58" t="s">
+        <v>667</v>
+      </c>
+      <c r="K58" t="b">
+        <v>1</v>
+      </c>
+      <c r="L58" t="s">
         <v>247</v>
       </c>
-      <c r="J58" t="s">
+      <c r="M58" t="s">
         <v>248</v>
       </c>
-      <c r="K58" t="s">
+      <c r="N58" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>250</v>
       </c>
@@ -4594,14 +5149,23 @@
       <c r="H59" t="b">
         <v>1</v>
       </c>
-      <c r="I59" t="s">
+      <c r="I59" t="b">
+        <v>1</v>
+      </c>
+      <c r="J59" t="s">
+        <v>667</v>
+      </c>
+      <c r="K59" t="b">
+        <v>1</v>
+      </c>
+      <c r="L59" t="s">
         <v>252</v>
       </c>
-      <c r="J59" t="s">
+      <c r="M59" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>253</v>
       </c>
@@ -4626,14 +5190,23 @@
       <c r="H60" t="b">
         <v>1</v>
       </c>
-      <c r="I60" t="s">
+      <c r="I60" t="b">
+        <v>1</v>
+      </c>
+      <c r="J60" t="s">
+        <v>667</v>
+      </c>
+      <c r="K60" t="b">
+        <v>1</v>
+      </c>
+      <c r="L60" t="s">
         <v>252</v>
       </c>
-      <c r="J60" t="s">
+      <c r="M60" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>255</v>
       </c>
@@ -4652,17 +5225,26 @@
       <c r="H61" t="b">
         <v>1</v>
       </c>
-      <c r="I61" t="s">
+      <c r="I61" t="b">
+        <v>1</v>
+      </c>
+      <c r="J61" t="s">
+        <v>668</v>
+      </c>
+      <c r="K61" t="b">
+        <v>1</v>
+      </c>
+      <c r="L61" t="s">
         <v>257</v>
       </c>
-      <c r="J61" t="s">
+      <c r="M61" t="s">
         <v>258</v>
       </c>
-      <c r="K61" t="s">
+      <c r="N61" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>260</v>
       </c>
@@ -4681,17 +5263,26 @@
       <c r="H62" t="b">
         <v>1</v>
       </c>
-      <c r="I62" t="s">
+      <c r="I62" t="b">
+        <v>1</v>
+      </c>
+      <c r="J62" t="s">
+        <v>668</v>
+      </c>
+      <c r="K62" t="b">
+        <v>1</v>
+      </c>
+      <c r="L62" t="s">
         <v>262</v>
       </c>
-      <c r="J62" t="s">
+      <c r="M62" t="s">
         <v>263</v>
       </c>
-      <c r="K62" t="s">
+      <c r="N62" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>265</v>
       </c>
@@ -4713,17 +5304,26 @@
       <c r="H63" t="b">
         <v>1</v>
       </c>
-      <c r="I63" t="s">
+      <c r="I63" t="b">
+        <v>1</v>
+      </c>
+      <c r="J63" t="s">
+        <v>668</v>
+      </c>
+      <c r="K63" t="b">
+        <v>1</v>
+      </c>
+      <c r="L63" t="s">
         <v>267</v>
       </c>
-      <c r="J63" t="s">
+      <c r="M63" t="s">
         <v>268</v>
       </c>
-      <c r="K63">
+      <c r="N63">
         <v>14</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>269</v>
       </c>
@@ -4742,14 +5342,23 @@
       <c r="H64" t="b">
         <v>1</v>
       </c>
-      <c r="I64" t="s">
+      <c r="I64" t="b">
+        <v>1</v>
+      </c>
+      <c r="J64" t="s">
+        <v>668</v>
+      </c>
+      <c r="K64" t="b">
+        <v>1</v>
+      </c>
+      <c r="L64" t="s">
         <v>271</v>
       </c>
-      <c r="J64" t="s">
+      <c r="M64" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>272</v>
       </c>
@@ -4768,14 +5377,23 @@
       <c r="H65" t="b">
         <v>1</v>
       </c>
-      <c r="I65" t="s">
+      <c r="I65" t="b">
+        <v>1</v>
+      </c>
+      <c r="J65" t="s">
+        <v>668</v>
+      </c>
+      <c r="K65" t="b">
+        <v>1</v>
+      </c>
+      <c r="L65" t="s">
         <v>271</v>
       </c>
-      <c r="J65" t="s">
+      <c r="M65" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>274</v>
       </c>
@@ -4794,17 +5412,26 @@
       <c r="H66" t="b">
         <v>1</v>
       </c>
-      <c r="I66" t="s">
+      <c r="I66" t="b">
+        <v>1</v>
+      </c>
+      <c r="J66" t="s">
+        <v>668</v>
+      </c>
+      <c r="K66" t="b">
+        <v>1</v>
+      </c>
+      <c r="L66" t="s">
         <v>276</v>
       </c>
-      <c r="J66" t="s">
+      <c r="M66" t="s">
         <v>277</v>
       </c>
-      <c r="K66" t="s">
+      <c r="N66" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>279</v>
       </c>
@@ -4823,17 +5450,26 @@
       <c r="H67" t="b">
         <v>1</v>
       </c>
-      <c r="I67" t="s">
+      <c r="I67" t="b">
+        <v>1</v>
+      </c>
+      <c r="J67" t="s">
+        <v>668</v>
+      </c>
+      <c r="K67" t="b">
+        <v>1</v>
+      </c>
+      <c r="L67" t="s">
         <v>281</v>
       </c>
-      <c r="J67" t="s">
+      <c r="M67" t="s">
         <v>282</v>
       </c>
-      <c r="K67" t="s">
+      <c r="N67" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>284</v>
       </c>
@@ -4855,17 +5491,26 @@
       <c r="H68" t="b">
         <v>1</v>
       </c>
-      <c r="I68" t="s">
+      <c r="I68" t="b">
+        <v>1</v>
+      </c>
+      <c r="J68" t="s">
+        <v>668</v>
+      </c>
+      <c r="K68" t="b">
+        <v>1</v>
+      </c>
+      <c r="L68" t="s">
         <v>287</v>
       </c>
-      <c r="J68" t="s">
+      <c r="M68" t="s">
         <v>288</v>
       </c>
-      <c r="K68" t="s">
+      <c r="N68" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>290</v>
       </c>
@@ -4884,14 +5529,23 @@
       <c r="H69" t="b">
         <v>1</v>
       </c>
-      <c r="I69" t="s">
+      <c r="I69" t="b">
+        <v>1</v>
+      </c>
+      <c r="J69" t="s">
+        <v>668</v>
+      </c>
+      <c r="K69" t="b">
+        <v>1</v>
+      </c>
+      <c r="L69" t="s">
         <v>292</v>
       </c>
-      <c r="J69" t="s">
+      <c r="M69" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>293</v>
       </c>
@@ -4916,14 +5570,23 @@
       <c r="H70" t="b">
         <v>1</v>
       </c>
-      <c r="I70" t="s">
+      <c r="I70" t="b">
+        <v>1</v>
+      </c>
+      <c r="J70" t="s">
+        <v>667</v>
+      </c>
+      <c r="K70" t="b">
+        <v>1</v>
+      </c>
+      <c r="L70" t="s">
         <v>292</v>
       </c>
-      <c r="J70" t="s">
+      <c r="M70" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>295</v>
       </c>
@@ -4948,17 +5611,26 @@
       <c r="H71" t="b">
         <v>1</v>
       </c>
-      <c r="I71" t="s">
+      <c r="I71" t="b">
+        <v>1</v>
+      </c>
+      <c r="J71" t="s">
+        <v>668</v>
+      </c>
+      <c r="K71" t="b">
+        <v>1</v>
+      </c>
+      <c r="L71" t="s">
         <v>297</v>
       </c>
-      <c r="J71" t="s">
+      <c r="M71" t="s">
         <v>298</v>
       </c>
-      <c r="K71" t="s">
+      <c r="N71" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>300</v>
       </c>
@@ -4977,14 +5649,23 @@
       <c r="H72" t="b">
         <v>1</v>
       </c>
-      <c r="I72" t="s">
+      <c r="I72" t="b">
+        <v>1</v>
+      </c>
+      <c r="J72" t="s">
+        <v>668</v>
+      </c>
+      <c r="K72" t="b">
+        <v>1</v>
+      </c>
+      <c r="L72" t="s">
         <v>302</v>
       </c>
-      <c r="J72" t="s">
+      <c r="M72" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>303</v>
       </c>
@@ -5009,14 +5690,23 @@
       <c r="H73" t="b">
         <v>1</v>
       </c>
-      <c r="I73" t="s">
+      <c r="I73" t="b">
+        <v>1</v>
+      </c>
+      <c r="J73" t="s">
+        <v>668</v>
+      </c>
+      <c r="K73" t="b">
+        <v>1</v>
+      </c>
+      <c r="L73" t="s">
         <v>302</v>
       </c>
-      <c r="J73" t="s">
+      <c r="M73" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>305</v>
       </c>
@@ -5035,14 +5725,23 @@
       <c r="H74" t="b">
         <v>1</v>
       </c>
-      <c r="I74" t="s">
+      <c r="I74" t="b">
+        <v>1</v>
+      </c>
+      <c r="J74" t="s">
+        <v>668</v>
+      </c>
+      <c r="K74" t="b">
+        <v>1</v>
+      </c>
+      <c r="L74" t="s">
         <v>307</v>
       </c>
-      <c r="J74" t="s">
+      <c r="M74" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>309</v>
       </c>
@@ -5061,17 +5760,26 @@
       <c r="H75" t="b">
         <v>1</v>
       </c>
-      <c r="I75" t="s">
+      <c r="I75" t="b">
+        <v>1</v>
+      </c>
+      <c r="J75" t="s">
+        <v>668</v>
+      </c>
+      <c r="K75" t="b">
+        <v>1</v>
+      </c>
+      <c r="L75" t="s">
         <v>312</v>
       </c>
-      <c r="J75" t="s">
+      <c r="M75" t="s">
         <v>313</v>
       </c>
-      <c r="K75">
+      <c r="N75">
         <v>1000000</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>314</v>
       </c>
@@ -5090,17 +5798,26 @@
       <c r="H76" t="b">
         <v>1</v>
       </c>
-      <c r="I76" t="s">
+      <c r="I76" t="b">
+        <v>1</v>
+      </c>
+      <c r="J76" t="s">
+        <v>668</v>
+      </c>
+      <c r="K76" t="b">
+        <v>1</v>
+      </c>
+      <c r="L76" t="s">
         <v>316</v>
       </c>
-      <c r="J76" t="s">
+      <c r="M76" t="s">
         <v>317</v>
       </c>
-      <c r="K76">
+      <c r="N76">
         <v>50000</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>318</v>
       </c>
@@ -5119,17 +5836,26 @@
       <c r="H77" t="b">
         <v>1</v>
       </c>
-      <c r="I77" t="s">
+      <c r="I77" t="b">
+        <v>1</v>
+      </c>
+      <c r="J77" t="s">
+        <v>668</v>
+      </c>
+      <c r="K77" t="b">
+        <v>1</v>
+      </c>
+      <c r="L77" t="s">
         <v>320</v>
       </c>
-      <c r="J77" t="s">
+      <c r="M77" t="s">
         <v>321</v>
       </c>
-      <c r="K77" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N77" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>322</v>
       </c>
@@ -5148,17 +5874,26 @@
       <c r="H78" t="b">
         <v>1</v>
       </c>
-      <c r="I78" t="s">
+      <c r="I78" t="b">
+        <v>1</v>
+      </c>
+      <c r="J78" t="s">
+        <v>668</v>
+      </c>
+      <c r="K78" t="b">
+        <v>1</v>
+      </c>
+      <c r="L78" t="s">
         <v>324</v>
       </c>
-      <c r="J78" t="s">
+      <c r="M78" t="s">
         <v>325</v>
       </c>
-      <c r="K78" t="s">
+      <c r="N78" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="79" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>327</v>
       </c>
@@ -5177,17 +5912,26 @@
       <c r="H79" t="b">
         <v>1</v>
       </c>
-      <c r="I79" t="s">
+      <c r="I79" t="b">
+        <v>1</v>
+      </c>
+      <c r="J79" t="s">
+        <v>668</v>
+      </c>
+      <c r="K79" t="b">
+        <v>1</v>
+      </c>
+      <c r="L79" t="s">
         <v>329</v>
       </c>
-      <c r="J79" t="s">
+      <c r="M79" t="s">
         <v>330</v>
       </c>
-      <c r="K79" s="1" t="s">
+      <c r="N79" s="1" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="80" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>332</v>
       </c>
@@ -5206,17 +5950,26 @@
       <c r="H80" t="b">
         <v>1</v>
       </c>
-      <c r="I80" t="s">
+      <c r="I80" t="b">
+        <v>1</v>
+      </c>
+      <c r="J80" t="s">
+        <v>668</v>
+      </c>
+      <c r="K80" t="b">
+        <v>1</v>
+      </c>
+      <c r="L80" t="s">
         <v>334</v>
       </c>
-      <c r="J80" s="1" t="s">
+      <c r="M80" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="K80" t="s">
+      <c r="N80" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="81" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>337</v>
       </c>
@@ -5241,17 +5994,26 @@
       <c r="H81" t="b">
         <v>1</v>
       </c>
-      <c r="I81" t="s">
+      <c r="I81" t="b">
+        <v>1</v>
+      </c>
+      <c r="J81" t="s">
+        <v>667</v>
+      </c>
+      <c r="K81" t="b">
+        <v>1</v>
+      </c>
+      <c r="L81" t="s">
         <v>340</v>
       </c>
-      <c r="J81" s="1" t="s">
+      <c r="M81" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="K81" t="s">
+      <c r="N81" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>343</v>
       </c>
@@ -5270,17 +6032,26 @@
       <c r="H82" t="b">
         <v>1</v>
       </c>
-      <c r="I82" t="s">
+      <c r="I82" t="b">
+        <v>1</v>
+      </c>
+      <c r="J82" t="s">
+        <v>668</v>
+      </c>
+      <c r="K82" t="b">
+        <v>1</v>
+      </c>
+      <c r="L82" t="s">
         <v>345</v>
       </c>
-      <c r="J82" t="s">
+      <c r="M82" t="s">
         <v>346</v>
       </c>
-      <c r="K82" t="s">
+      <c r="N82" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>348</v>
       </c>
@@ -5299,17 +6070,26 @@
       <c r="H83" t="b">
         <v>1</v>
       </c>
-      <c r="I83" t="s">
+      <c r="I83" t="b">
+        <v>1</v>
+      </c>
+      <c r="J83" t="s">
+        <v>668</v>
+      </c>
+      <c r="K83" t="b">
+        <v>1</v>
+      </c>
+      <c r="L83" t="s">
         <v>350</v>
       </c>
-      <c r="J83" t="s">
+      <c r="M83" t="s">
         <v>351</v>
       </c>
-      <c r="K83">
+      <c r="N83">
         <v>1000</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>352</v>
       </c>
@@ -5328,14 +6108,23 @@
       <c r="H84" t="b">
         <v>1</v>
       </c>
-      <c r="I84" t="s">
+      <c r="I84" t="b">
+        <v>1</v>
+      </c>
+      <c r="J84" t="s">
+        <v>668</v>
+      </c>
+      <c r="K84" t="b">
+        <v>1</v>
+      </c>
+      <c r="L84" t="s">
         <v>354</v>
       </c>
-      <c r="J84" t="s">
+      <c r="M84" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>355</v>
       </c>
@@ -5354,14 +6143,23 @@
       <c r="H85" t="b">
         <v>1</v>
       </c>
-      <c r="I85" t="s">
+      <c r="I85" t="b">
+        <v>1</v>
+      </c>
+      <c r="J85" t="s">
+        <v>668</v>
+      </c>
+      <c r="K85" t="b">
+        <v>1</v>
+      </c>
+      <c r="L85" t="s">
         <v>354</v>
       </c>
-      <c r="J85" t="s">
+      <c r="M85" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>357</v>
       </c>
@@ -5386,17 +6184,26 @@
       <c r="H86" t="b">
         <v>1</v>
       </c>
-      <c r="I86" t="s">
+      <c r="I86" t="b">
+        <v>1</v>
+      </c>
+      <c r="J86" t="s">
+        <v>668</v>
+      </c>
+      <c r="K86" t="b">
+        <v>1</v>
+      </c>
+      <c r="L86" t="s">
         <v>359</v>
       </c>
-      <c r="J86" t="s">
+      <c r="M86" t="s">
         <v>360</v>
       </c>
-      <c r="K86" t="s">
+      <c r="N86" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>362</v>
       </c>
@@ -5415,17 +6222,26 @@
       <c r="H87" t="b">
         <v>1</v>
       </c>
-      <c r="I87" t="s">
+      <c r="I87" t="b">
+        <v>1</v>
+      </c>
+      <c r="J87" t="s">
+        <v>668</v>
+      </c>
+      <c r="K87" t="b">
+        <v>1</v>
+      </c>
+      <c r="L87" t="s">
         <v>364</v>
       </c>
-      <c r="J87" t="s">
+      <c r="M87" t="s">
         <v>365</v>
       </c>
-      <c r="K87" t="s">
+      <c r="N87" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>367</v>
       </c>
@@ -5444,17 +6260,26 @@
       <c r="H88" t="b">
         <v>1</v>
       </c>
-      <c r="I88" t="s">
+      <c r="I88" t="b">
+        <v>1</v>
+      </c>
+      <c r="J88" t="s">
+        <v>668</v>
+      </c>
+      <c r="K88" t="b">
+        <v>1</v>
+      </c>
+      <c r="L88" t="s">
         <v>369</v>
       </c>
-      <c r="J88" t="s">
+      <c r="M88" t="s">
         <v>370</v>
       </c>
-      <c r="K88" t="s">
+      <c r="N88" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="89" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>372</v>
       </c>
@@ -5479,17 +6304,26 @@
       <c r="H89" t="b">
         <v>1</v>
       </c>
-      <c r="I89" t="s">
+      <c r="I89" t="b">
+        <v>1</v>
+      </c>
+      <c r="J89" t="s">
+        <v>667</v>
+      </c>
+      <c r="K89" t="b">
+        <v>1</v>
+      </c>
+      <c r="L89" t="s">
         <v>374</v>
       </c>
-      <c r="J89" s="1" t="s">
+      <c r="M89" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="K89" t="s">
+      <c r="N89" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>377</v>
       </c>
@@ -5514,17 +6348,26 @@
       <c r="H90" t="b">
         <v>1</v>
       </c>
-      <c r="I90" t="s">
+      <c r="I90" t="b">
+        <v>1</v>
+      </c>
+      <c r="J90" t="s">
+        <v>668</v>
+      </c>
+      <c r="K90" t="b">
+        <v>1</v>
+      </c>
+      <c r="L90" t="s">
         <v>379</v>
       </c>
-      <c r="J90" t="s">
+      <c r="M90" t="s">
         <v>380</v>
       </c>
-      <c r="K90" t="s">
+      <c r="N90" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>382</v>
       </c>
@@ -5549,17 +6392,26 @@
       <c r="H91" t="b">
         <v>1</v>
       </c>
-      <c r="I91" t="s">
+      <c r="I91" t="b">
+        <v>1</v>
+      </c>
+      <c r="J91" t="s">
+        <v>668</v>
+      </c>
+      <c r="K91" t="b">
+        <v>1</v>
+      </c>
+      <c r="L91" t="s">
         <v>384</v>
       </c>
-      <c r="J91" t="s">
+      <c r="M91" t="s">
         <v>385</v>
       </c>
-      <c r="K91" t="s">
+      <c r="N91" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="92" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:14" ht="105" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>387</v>
       </c>
@@ -5578,17 +6430,26 @@
       <c r="H92" t="b">
         <v>1</v>
       </c>
-      <c r="I92" t="s">
+      <c r="I92" t="b">
+        <v>1</v>
+      </c>
+      <c r="J92" t="s">
+        <v>668</v>
+      </c>
+      <c r="K92" t="b">
+        <v>1</v>
+      </c>
+      <c r="L92" t="s">
         <v>389</v>
       </c>
-      <c r="J92" s="1" t="s">
+      <c r="M92" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="K92" t="s">
+      <c r="N92" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="93" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:14" ht="90" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>392</v>
       </c>
@@ -5607,17 +6468,26 @@
       <c r="H93" t="b">
         <v>1</v>
       </c>
-      <c r="I93" t="s">
+      <c r="I93" t="b">
+        <v>1</v>
+      </c>
+      <c r="J93" t="s">
+        <v>668</v>
+      </c>
+      <c r="K93" t="b">
+        <v>1</v>
+      </c>
+      <c r="L93" t="s">
         <v>394</v>
       </c>
-      <c r="J93" s="1" t="s">
+      <c r="M93" s="1" t="s">
         <v>395</v>
       </c>
-      <c r="K93" t="s">
+      <c r="N93" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>397</v>
       </c>
@@ -5636,17 +6506,26 @@
       <c r="H94" t="b">
         <v>1</v>
       </c>
-      <c r="I94" t="s">
+      <c r="I94" t="b">
+        <v>1</v>
+      </c>
+      <c r="J94" t="s">
+        <v>667</v>
+      </c>
+      <c r="K94" t="b">
+        <v>1</v>
+      </c>
+      <c r="L94" t="s">
         <v>400</v>
       </c>
-      <c r="J94" t="s">
+      <c r="M94" t="s">
         <v>401</v>
       </c>
-      <c r="K94" t="s">
+      <c r="N94" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>403</v>
       </c>
@@ -5665,17 +6544,26 @@
       <c r="H95" t="b">
         <v>1</v>
       </c>
-      <c r="I95" t="s">
+      <c r="I95" t="b">
+        <v>1</v>
+      </c>
+      <c r="J95" t="s">
+        <v>667</v>
+      </c>
+      <c r="K95" t="b">
+        <v>1</v>
+      </c>
+      <c r="L95" t="s">
         <v>405</v>
       </c>
-      <c r="J95" t="s">
+      <c r="M95" t="s">
         <v>406</v>
       </c>
-      <c r="K95">
+      <c r="N95">
         <v>10365118</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>407</v>
       </c>
@@ -5700,17 +6588,26 @@
       <c r="H96" t="b">
         <v>1</v>
       </c>
-      <c r="I96" t="s">
+      <c r="I96" t="b">
+        <v>1</v>
+      </c>
+      <c r="J96" t="s">
+        <v>668</v>
+      </c>
+      <c r="K96" t="b">
+        <v>1</v>
+      </c>
+      <c r="L96" t="s">
         <v>409</v>
       </c>
-      <c r="J96" t="s">
+      <c r="M96" t="s">
         <v>410</v>
       </c>
-      <c r="K96" t="s">
+      <c r="N96" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>412</v>
       </c>
@@ -5729,17 +6626,26 @@
       <c r="H97" t="b">
         <v>1</v>
       </c>
-      <c r="I97" t="s">
+      <c r="I97" t="b">
+        <v>1</v>
+      </c>
+      <c r="J97" t="s">
+        <v>668</v>
+      </c>
+      <c r="K97" t="b">
+        <v>1</v>
+      </c>
+      <c r="L97" t="s">
         <v>414</v>
       </c>
-      <c r="J97" t="s">
+      <c r="M97" t="s">
         <v>415</v>
       </c>
-      <c r="K97" t="s">
+      <c r="N97" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>417</v>
       </c>
@@ -5758,17 +6664,26 @@
       <c r="H98" t="b">
         <v>1</v>
       </c>
-      <c r="I98" t="s">
+      <c r="I98" t="b">
+        <v>1</v>
+      </c>
+      <c r="J98" t="s">
+        <v>667</v>
+      </c>
+      <c r="K98" t="b">
+        <v>1</v>
+      </c>
+      <c r="L98" t="s">
         <v>419</v>
       </c>
-      <c r="J98" t="s">
+      <c r="M98" t="s">
         <v>419</v>
       </c>
-      <c r="K98" s="2">
+      <c r="N98" s="2">
         <v>42720</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>420</v>
       </c>
@@ -5787,17 +6702,26 @@
       <c r="H99" t="b">
         <v>1</v>
       </c>
-      <c r="I99" t="s">
+      <c r="I99" t="b">
+        <v>1</v>
+      </c>
+      <c r="J99" t="s">
+        <v>668</v>
+      </c>
+      <c r="K99" t="b">
+        <v>1</v>
+      </c>
+      <c r="L99" t="s">
         <v>422</v>
       </c>
-      <c r="J99" t="s">
+      <c r="M99" t="s">
         <v>423</v>
       </c>
-      <c r="K99" t="s">
+      <c r="N99" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>425</v>
       </c>
@@ -5816,14 +6740,23 @@
       <c r="H100" t="b">
         <v>1</v>
       </c>
-      <c r="I100" t="s">
+      <c r="I100" t="b">
+        <v>1</v>
+      </c>
+      <c r="J100" t="s">
+        <v>668</v>
+      </c>
+      <c r="K100" t="b">
+        <v>1</v>
+      </c>
+      <c r="L100" t="s">
         <v>427</v>
       </c>
-      <c r="J100" t="s">
+      <c r="M100" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>429</v>
       </c>
@@ -5842,17 +6775,26 @@
       <c r="H101" t="b">
         <v>1</v>
       </c>
-      <c r="I101" t="s">
+      <c r="I101" t="b">
+        <v>1</v>
+      </c>
+      <c r="J101" t="s">
+        <v>668</v>
+      </c>
+      <c r="K101" t="b">
+        <v>1</v>
+      </c>
+      <c r="L101" t="s">
         <v>431</v>
       </c>
-      <c r="J101" t="s">
+      <c r="M101" t="s">
         <v>432</v>
       </c>
-      <c r="K101" t="s">
+      <c r="N101" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>434</v>
       </c>
@@ -5871,17 +6813,26 @@
       <c r="H102" t="b">
         <v>1</v>
       </c>
-      <c r="I102" t="s">
+      <c r="I102" t="b">
+        <v>1</v>
+      </c>
+      <c r="J102" t="s">
+        <v>667</v>
+      </c>
+      <c r="K102" t="b">
+        <v>1</v>
+      </c>
+      <c r="L102" t="s">
         <v>436</v>
       </c>
-      <c r="J102" t="s">
+      <c r="M102" t="s">
         <v>437</v>
       </c>
-      <c r="K102" t="s">
+      <c r="N102" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>439</v>
       </c>
@@ -5906,17 +6857,26 @@
       <c r="H103" t="b">
         <v>1</v>
       </c>
-      <c r="I103" t="s">
+      <c r="I103" t="b">
+        <v>1</v>
+      </c>
+      <c r="J103" t="s">
+        <v>668</v>
+      </c>
+      <c r="K103" t="b">
+        <v>1</v>
+      </c>
+      <c r="L103" t="s">
         <v>441</v>
       </c>
-      <c r="J103" t="s">
+      <c r="M103" t="s">
         <v>442</v>
       </c>
-      <c r="K103">
+      <c r="N103">
         <v>300</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>443</v>
       </c>
@@ -5935,17 +6895,26 @@
       <c r="H104" t="b">
         <v>1</v>
       </c>
-      <c r="I104" t="s">
+      <c r="I104" t="b">
+        <v>1</v>
+      </c>
+      <c r="J104" t="s">
+        <v>668</v>
+      </c>
+      <c r="K104" t="b">
+        <v>1</v>
+      </c>
+      <c r="L104" t="s">
         <v>445</v>
       </c>
-      <c r="J104" t="s">
+      <c r="M104" t="s">
         <v>446</v>
       </c>
-      <c r="K104" t="s">
+      <c r="N104" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>448</v>
       </c>
@@ -5964,17 +6933,26 @@
       <c r="H105" t="b">
         <v>1</v>
       </c>
-      <c r="I105" t="s">
+      <c r="I105" t="b">
+        <v>1</v>
+      </c>
+      <c r="J105" t="s">
+        <v>668</v>
+      </c>
+      <c r="K105" t="b">
+        <v>1</v>
+      </c>
+      <c r="L105" t="s">
         <v>450</v>
       </c>
-      <c r="J105" t="s">
+      <c r="M105" t="s">
         <v>451</v>
       </c>
-      <c r="K105" t="s">
+      <c r="N105" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>453</v>
       </c>
@@ -5993,17 +6971,26 @@
       <c r="H106" t="b">
         <v>1</v>
       </c>
-      <c r="I106" t="s">
+      <c r="I106" t="b">
+        <v>1</v>
+      </c>
+      <c r="J106" t="s">
+        <v>668</v>
+      </c>
+      <c r="K106" t="b">
+        <v>1</v>
+      </c>
+      <c r="L106" t="s">
         <v>455</v>
       </c>
-      <c r="J106" t="s">
+      <c r="M106" t="s">
         <v>456</v>
       </c>
-      <c r="K106">
+      <c r="N106">
         <v>300</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>457</v>
       </c>
@@ -6022,14 +7009,23 @@
       <c r="H107" t="b">
         <v>1</v>
       </c>
-      <c r="I107" t="s">
+      <c r="I107" t="b">
+        <v>1</v>
+      </c>
+      <c r="J107" t="s">
+        <v>668</v>
+      </c>
+      <c r="K107" t="b">
+        <v>1</v>
+      </c>
+      <c r="L107" t="s">
         <v>460</v>
       </c>
-      <c r="J107" t="s">
+      <c r="M107" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="108" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>462</v>
       </c>
@@ -6048,14 +7044,23 @@
       <c r="H108" t="b">
         <v>1</v>
       </c>
-      <c r="I108" t="s">
+      <c r="I108" t="b">
+        <v>1</v>
+      </c>
+      <c r="J108" t="s">
+        <v>668</v>
+      </c>
+      <c r="K108" t="b">
+        <v>1</v>
+      </c>
+      <c r="L108" t="s">
         <v>464</v>
       </c>
-      <c r="J108" s="1" t="s">
+      <c r="M108" s="1" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>466</v>
       </c>
@@ -6074,17 +7079,26 @@
       <c r="H109" t="b">
         <v>1</v>
       </c>
-      <c r="I109" t="s">
+      <c r="I109" t="b">
+        <v>1</v>
+      </c>
+      <c r="J109" t="s">
+        <v>668</v>
+      </c>
+      <c r="K109" t="b">
+        <v>1</v>
+      </c>
+      <c r="L109" t="s">
         <v>468</v>
       </c>
-      <c r="J109" t="s">
+      <c r="M109" t="s">
         <v>469</v>
       </c>
-      <c r="K109" t="s">
+      <c r="N109" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>471</v>
       </c>
@@ -6103,17 +7117,26 @@
       <c r="H110" t="b">
         <v>1</v>
       </c>
-      <c r="I110" t="s">
+      <c r="I110" t="b">
+        <v>1</v>
+      </c>
+      <c r="J110" t="s">
+        <v>668</v>
+      </c>
+      <c r="K110" t="b">
+        <v>1</v>
+      </c>
+      <c r="L110" t="s">
         <v>473</v>
       </c>
-      <c r="J110" t="s">
+      <c r="M110" t="s">
         <v>474</v>
       </c>
-      <c r="K110" t="s">
+      <c r="N110" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>476</v>
       </c>
@@ -6132,17 +7155,26 @@
       <c r="H111" t="b">
         <v>1</v>
       </c>
-      <c r="I111" t="s">
+      <c r="I111" t="b">
+        <v>1</v>
+      </c>
+      <c r="J111" t="s">
+        <v>668</v>
+      </c>
+      <c r="K111" t="b">
+        <v>1</v>
+      </c>
+      <c r="L111" t="s">
         <v>478</v>
       </c>
-      <c r="J111" t="s">
+      <c r="M111" t="s">
         <v>479</v>
       </c>
-      <c r="K111" t="s">
+      <c r="N111" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>481</v>
       </c>
@@ -6161,17 +7193,26 @@
       <c r="H112" t="b">
         <v>1</v>
       </c>
-      <c r="I112" t="s">
+      <c r="I112" t="b">
+        <v>1</v>
+      </c>
+      <c r="J112" t="s">
+        <v>668</v>
+      </c>
+      <c r="K112" t="b">
+        <v>1</v>
+      </c>
+      <c r="L112" t="s">
         <v>483</v>
       </c>
-      <c r="J112" t="s">
+      <c r="M112" t="s">
         <v>484</v>
       </c>
-      <c r="K112" t="s">
+      <c r="N112" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>486</v>
       </c>
@@ -6190,17 +7231,26 @@
       <c r="H113" t="b">
         <v>1</v>
       </c>
-      <c r="I113" t="s">
+      <c r="I113" t="b">
+        <v>1</v>
+      </c>
+      <c r="J113" t="s">
+        <v>668</v>
+      </c>
+      <c r="K113" t="b">
+        <v>1</v>
+      </c>
+      <c r="L113" t="s">
         <v>488</v>
       </c>
-      <c r="J113" t="s">
+      <c r="M113" t="s">
         <v>489</v>
       </c>
-      <c r="K113" t="s">
+      <c r="N113" t="s">
         <v>490</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>491</v>
       </c>
@@ -6219,17 +7269,26 @@
       <c r="H114" t="b">
         <v>1</v>
       </c>
-      <c r="I114" t="s">
+      <c r="I114" t="b">
+        <v>1</v>
+      </c>
+      <c r="J114" t="s">
+        <v>668</v>
+      </c>
+      <c r="K114" t="b">
+        <v>1</v>
+      </c>
+      <c r="L114" t="s">
         <v>493</v>
       </c>
-      <c r="J114" t="s">
+      <c r="M114" t="s">
         <v>494</v>
       </c>
-      <c r="K114" t="s">
+      <c r="N114" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>496</v>
       </c>
@@ -6248,11 +7307,20 @@
       <c r="H115" t="b">
         <v>1</v>
       </c>
-      <c r="I115" t="s">
+      <c r="I115" t="b">
+        <v>1</v>
+      </c>
+      <c r="J115" t="s">
+        <v>668</v>
+      </c>
+      <c r="K115" t="b">
+        <v>1</v>
+      </c>
+      <c r="L115" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>499</v>
       </c>
@@ -6271,17 +7339,26 @@
       <c r="H116" t="b">
         <v>1</v>
       </c>
-      <c r="I116" t="s">
+      <c r="I116" t="b">
+        <v>1</v>
+      </c>
+      <c r="J116" t="s">
+        <v>668</v>
+      </c>
+      <c r="K116" t="b">
+        <v>1</v>
+      </c>
+      <c r="L116" t="s">
         <v>501</v>
       </c>
-      <c r="J116" t="s">
+      <c r="M116" t="s">
         <v>502</v>
       </c>
-      <c r="K116" t="s">
+      <c r="N116" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>504</v>
       </c>
@@ -6300,14 +7377,23 @@
       <c r="H117" t="b">
         <v>1</v>
       </c>
-      <c r="I117" t="s">
+      <c r="I117" t="b">
+        <v>1</v>
+      </c>
+      <c r="J117" t="s">
+        <v>668</v>
+      </c>
+      <c r="K117" t="b">
+        <v>1</v>
+      </c>
+      <c r="L117" t="s">
         <v>506</v>
       </c>
-      <c r="J117" t="s">
+      <c r="M117" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
         <v>545</v>
       </c>
@@ -6324,19 +7410,28 @@
         <v>311</v>
       </c>
       <c r="H118" t="b">
+        <v>1</v>
+      </c>
+      <c r="I118" t="b">
+        <v>1</v>
+      </c>
+      <c r="J118" t="s">
+        <v>667</v>
+      </c>
+      <c r="K118" t="b">
         <v>0</v>
       </c>
-      <c r="I118" t="s">
+      <c r="L118" t="s">
         <v>556</v>
       </c>
-      <c r="J118" t="s">
+      <c r="M118" t="s">
         <v>554</v>
       </c>
-      <c r="L118" t="s">
+      <c r="O118" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
         <v>546</v>
       </c>
@@ -6353,19 +7448,28 @@
         <v>311</v>
       </c>
       <c r="H119" t="b">
+        <v>1</v>
+      </c>
+      <c r="I119" t="b">
+        <v>1</v>
+      </c>
+      <c r="J119" t="s">
+        <v>667</v>
+      </c>
+      <c r="K119" t="b">
         <v>0</v>
       </c>
-      <c r="I119" t="s">
+      <c r="L119" t="s">
         <v>557</v>
       </c>
-      <c r="J119" t="s">
+      <c r="M119" t="s">
         <v>555</v>
       </c>
-      <c r="L119" t="s">
+      <c r="O119" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="120" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
         <v>547</v>
       </c>
@@ -6379,19 +7483,28 @@
         <v>11</v>
       </c>
       <c r="H120" t="b">
+        <v>1</v>
+      </c>
+      <c r="I120" t="b">
+        <v>1</v>
+      </c>
+      <c r="J120" t="s">
+        <v>668</v>
+      </c>
+      <c r="K120" t="b">
         <v>0</v>
       </c>
-      <c r="I120" t="s">
+      <c r="L120" t="s">
         <v>558</v>
       </c>
-      <c r="J120" s="1" t="s">
+      <c r="M120" s="1" t="s">
         <v>559</v>
       </c>
-      <c r="L120" t="s">
+      <c r="O120" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
         <v>548</v>
       </c>
@@ -6408,19 +7521,28 @@
         <v>11</v>
       </c>
       <c r="H121" t="b">
+        <v>1</v>
+      </c>
+      <c r="I121" t="b">
+        <v>1</v>
+      </c>
+      <c r="J121" t="s">
+        <v>668</v>
+      </c>
+      <c r="K121" t="b">
         <v>0</v>
       </c>
-      <c r="I121" t="s">
+      <c r="L121" t="s">
         <v>560</v>
       </c>
-      <c r="J121" t="s">
+      <c r="M121" t="s">
         <v>561</v>
       </c>
-      <c r="L121" t="s">
+      <c r="O121" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
         <v>661</v>
       </c>
@@ -6437,19 +7559,28 @@
         <v>11</v>
       </c>
       <c r="H122" t="b">
+        <v>1</v>
+      </c>
+      <c r="I122" t="b">
+        <v>1</v>
+      </c>
+      <c r="J122" t="s">
+        <v>667</v>
+      </c>
+      <c r="K122" t="b">
         <v>0</v>
       </c>
-      <c r="I122" t="s">
+      <c r="L122" t="s">
         <v>562</v>
       </c>
-      <c r="J122" t="s">
+      <c r="M122" t="s">
         <v>563</v>
       </c>
-      <c r="L122" t="s">
+      <c r="O122" t="s">
         <v>529</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
         <v>550</v>
       </c>
@@ -6465,17 +7596,26 @@
       <c r="H123" t="b">
         <v>0</v>
       </c>
-      <c r="I123" t="s">
+      <c r="I123" t="b">
+        <v>1</v>
+      </c>
+      <c r="J123" t="s">
+        <v>667</v>
+      </c>
+      <c r="K123" t="b">
+        <v>0</v>
+      </c>
+      <c r="L123" t="s">
         <v>564</v>
       </c>
-      <c r="J123" t="s">
+      <c r="M123" t="s">
         <v>565</v>
       </c>
-      <c r="L123" t="s">
+      <c r="O123" t="s">
         <v>551</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
         <v>663</v>
       </c>
@@ -6492,19 +7632,28 @@
         <v>11</v>
       </c>
       <c r="H124" t="b">
+        <v>1</v>
+      </c>
+      <c r="I124" t="b">
+        <v>1</v>
+      </c>
+      <c r="J124" t="s">
+        <v>667</v>
+      </c>
+      <c r="K124" t="b">
         <v>0</v>
       </c>
-      <c r="I124" t="s">
+      <c r="L124" t="s">
         <v>571</v>
       </c>
-      <c r="J124" t="s">
+      <c r="M124" t="s">
         <v>566</v>
       </c>
-      <c r="L124" t="s">
+      <c r="O124" t="s">
         <v>529</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
         <v>552</v>
       </c>
@@ -6521,19 +7670,28 @@
         <v>311</v>
       </c>
       <c r="H125" t="b">
+        <v>1</v>
+      </c>
+      <c r="I125" t="b">
+        <v>1</v>
+      </c>
+      <c r="J125" t="s">
+        <v>667</v>
+      </c>
+      <c r="K125" t="b">
         <v>0</v>
       </c>
-      <c r="I125" t="s">
+      <c r="L125" t="s">
         <v>648</v>
       </c>
-      <c r="J125" t="s">
+      <c r="M125" t="s">
         <v>649</v>
       </c>
-      <c r="L125" t="s">
+      <c r="O125" t="s">
         <v>529</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
         <v>553</v>
       </c>
@@ -6547,19 +7705,28 @@
         <v>11</v>
       </c>
       <c r="H126" t="b">
+        <v>1</v>
+      </c>
+      <c r="I126" t="b">
+        <v>1</v>
+      </c>
+      <c r="J126" t="s">
+        <v>668</v>
+      </c>
+      <c r="K126" t="b">
         <v>0</v>
       </c>
-      <c r="I126" t="s">
+      <c r="L126" t="s">
         <v>567</v>
       </c>
-      <c r="J126" t="s">
+      <c r="M126" t="s">
         <v>568</v>
       </c>
-      <c r="L126" t="s">
+      <c r="O126" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
         <v>652</v>
       </c>
@@ -6573,16 +7740,25 @@
         <v>11</v>
       </c>
       <c r="H127" t="b">
+        <v>1</v>
+      </c>
+      <c r="I127" t="b">
+        <v>1</v>
+      </c>
+      <c r="J127" t="s">
+        <v>668</v>
+      </c>
+      <c r="K127" t="b">
         <v>0</v>
       </c>
-      <c r="I127" t="s">
+      <c r="L127" t="s">
         <v>653</v>
       </c>
-      <c r="J127" t="s">
+      <c r="M127" t="s">
         <v>654</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
         <v>572</v>
       </c>
@@ -6599,19 +7775,28 @@
         <v>11</v>
       </c>
       <c r="H128" t="b">
+        <v>1</v>
+      </c>
+      <c r="I128" t="b">
+        <v>1</v>
+      </c>
+      <c r="J128" t="s">
+        <v>668</v>
+      </c>
+      <c r="K128" t="b">
         <v>0</v>
       </c>
-      <c r="I128" t="s">
+      <c r="L128" t="s">
         <v>569</v>
       </c>
-      <c r="J128" t="s">
+      <c r="M128" t="s">
         <v>569</v>
       </c>
-      <c r="L128" t="s">
+      <c r="O128" t="s">
         <v>537</v>
       </c>
     </row>
-    <row r="129" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
         <v>655</v>
       </c>
@@ -6627,14 +7812,23 @@
       <c r="H129" t="b">
         <v>0</v>
       </c>
-      <c r="I129" t="s">
+      <c r="I129" t="b">
+        <v>1</v>
+      </c>
+      <c r="J129" t="s">
+        <v>668</v>
+      </c>
+      <c r="K129" t="b">
+        <v>0</v>
+      </c>
+      <c r="L129" t="s">
         <v>656</v>
       </c>
-      <c r="J129" t="s">
+      <c r="M129" t="s">
         <v>657</v>
       </c>
     </row>
-    <row r="130" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
         <v>658</v>
       </c>
@@ -6650,14 +7844,23 @@
       <c r="H130" t="b">
         <v>0</v>
       </c>
-      <c r="I130" t="s">
+      <c r="I130" t="b">
+        <v>1</v>
+      </c>
+      <c r="J130" t="s">
+        <v>668</v>
+      </c>
+      <c r="K130" t="b">
+        <v>0</v>
+      </c>
+      <c r="L130" t="s">
         <v>567</v>
       </c>
-      <c r="J130" t="s">
+      <c r="M130" t="s">
         <v>659</v>
       </c>
     </row>
-    <row r="131" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
         <v>662</v>
       </c>
@@ -6671,16 +7874,25 @@
         <v>11</v>
       </c>
       <c r="H131" t="b">
+        <v>1</v>
+      </c>
+      <c r="I131" t="b">
+        <v>1</v>
+      </c>
+      <c r="J131" t="s">
+        <v>667</v>
+      </c>
+      <c r="K131" t="b">
         <v>0</v>
       </c>
-      <c r="I131" t="s">
+      <c r="L131" t="s">
         <v>570</v>
       </c>
-      <c r="J131" t="s">
+      <c r="M131" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="132" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
         <v>582</v>
       </c>
@@ -6697,19 +7909,28 @@
         <v>11</v>
       </c>
       <c r="H132" t="b">
+        <v>1</v>
+      </c>
+      <c r="I132" t="b">
+        <v>1</v>
+      </c>
+      <c r="J132" t="s">
+        <v>668</v>
+      </c>
+      <c r="K132" t="b">
         <v>0</v>
       </c>
-      <c r="I132" t="s">
+      <c r="L132" t="s">
         <v>590</v>
       </c>
-      <c r="J132" t="s">
+      <c r="M132" t="s">
         <v>590</v>
       </c>
-      <c r="K132" t="s">
+      <c r="N132" t="s">
         <v>601</v>
       </c>
     </row>
-    <row r="133" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
         <v>583</v>
       </c>
@@ -6726,19 +7947,28 @@
         <v>11</v>
       </c>
       <c r="H133" t="b">
+        <v>1</v>
+      </c>
+      <c r="I133" t="b">
+        <v>1</v>
+      </c>
+      <c r="J133" t="s">
+        <v>668</v>
+      </c>
+      <c r="K133" t="b">
         <v>0</v>
       </c>
-      <c r="I133" t="s">
+      <c r="L133" t="s">
         <v>591</v>
       </c>
-      <c r="J133" t="s">
+      <c r="M133" t="s">
         <v>591</v>
       </c>
-      <c r="K133" t="s">
+      <c r="N133" t="s">
         <v>602</v>
       </c>
     </row>
-    <row r="134" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
         <v>584</v>
       </c>
@@ -6755,19 +7985,28 @@
         <v>11</v>
       </c>
       <c r="H134" t="b">
+        <v>1</v>
+      </c>
+      <c r="I134" t="b">
+        <v>1</v>
+      </c>
+      <c r="J134" t="s">
+        <v>668</v>
+      </c>
+      <c r="K134" t="b">
         <v>0</v>
       </c>
-      <c r="I134" t="s">
+      <c r="L134" t="s">
         <v>593</v>
       </c>
-      <c r="J134" t="s">
+      <c r="M134" t="s">
         <v>593</v>
       </c>
-      <c r="K134">
+      <c r="N134">
         <v>1.18</v>
       </c>
     </row>
-    <row r="135" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
         <v>608</v>
       </c>
@@ -6784,19 +8023,28 @@
         <v>11</v>
       </c>
       <c r="H135" t="b">
+        <v>1</v>
+      </c>
+      <c r="I135" t="b">
+        <v>1</v>
+      </c>
+      <c r="J135" t="s">
+        <v>668</v>
+      </c>
+      <c r="K135" t="b">
         <v>0</v>
       </c>
-      <c r="I135" t="s">
+      <c r="L135" t="s">
         <v>643</v>
       </c>
-      <c r="J135" t="s">
+      <c r="M135" t="s">
         <v>643</v>
       </c>
-      <c r="K135" t="s">
+      <c r="N135" t="s">
         <v>642</v>
       </c>
     </row>
-    <row r="136" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B136" t="s">
         <v>609</v>
       </c>
@@ -6813,19 +8061,28 @@
         <v>11</v>
       </c>
       <c r="H136" t="b">
+        <v>1</v>
+      </c>
+      <c r="I136" t="b">
+        <v>1</v>
+      </c>
+      <c r="J136" t="s">
+        <v>668</v>
+      </c>
+      <c r="K136" t="b">
         <v>0</v>
       </c>
-      <c r="I136" t="s">
+      <c r="L136" t="s">
         <v>644</v>
       </c>
-      <c r="J136" t="s">
+      <c r="M136" t="s">
         <v>644</v>
       </c>
-      <c r="K136" t="s">
+      <c r="N136" t="s">
         <v>642</v>
       </c>
     </row>
-    <row r="137" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
         <v>610</v>
       </c>
@@ -6842,19 +8099,28 @@
         <v>11</v>
       </c>
       <c r="H137" t="b">
+        <v>1</v>
+      </c>
+      <c r="I137" t="b">
+        <v>1</v>
+      </c>
+      <c r="J137" t="s">
+        <v>668</v>
+      </c>
+      <c r="K137" t="b">
         <v>0</v>
       </c>
-      <c r="I137" t="s">
+      <c r="L137" t="s">
         <v>641</v>
       </c>
-      <c r="J137" t="s">
+      <c r="M137" t="s">
         <v>641</v>
       </c>
-      <c r="K137" t="s">
+      <c r="N137" t="s">
         <v>642</v>
       </c>
     </row>
-    <row r="138" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B138" t="s">
         <v>585</v>
       </c>
@@ -6871,19 +8137,28 @@
         <v>11</v>
       </c>
       <c r="H138" t="b">
+        <v>1</v>
+      </c>
+      <c r="I138" t="b">
+        <v>1</v>
+      </c>
+      <c r="J138" t="s">
+        <v>668</v>
+      </c>
+      <c r="K138" t="b">
         <v>0</v>
       </c>
-      <c r="I138" t="s">
+      <c r="L138" t="s">
         <v>594</v>
       </c>
-      <c r="J138" t="s">
+      <c r="M138" t="s">
         <v>594</v>
       </c>
-      <c r="K138" t="s">
+      <c r="N138" t="s">
         <v>600</v>
       </c>
     </row>
-    <row r="139" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B139" t="s">
         <v>586</v>
       </c>
@@ -6900,19 +8175,28 @@
         <v>11</v>
       </c>
       <c r="H139" t="b">
+        <v>1</v>
+      </c>
+      <c r="I139" t="b">
+        <v>1</v>
+      </c>
+      <c r="J139" t="s">
+        <v>668</v>
+      </c>
+      <c r="K139" t="b">
         <v>0</v>
       </c>
-      <c r="I139" t="s">
+      <c r="L139" t="s">
         <v>595</v>
       </c>
-      <c r="J139" t="s">
+      <c r="M139" t="s">
         <v>595</v>
       </c>
-      <c r="K139">
+      <c r="N139">
         <v>1.2</v>
       </c>
     </row>
-    <row r="140" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
         <v>587</v>
       </c>
@@ -6929,19 +8213,28 @@
         <v>11</v>
       </c>
       <c r="H140" t="b">
+        <v>1</v>
+      </c>
+      <c r="I140" t="b">
+        <v>1</v>
+      </c>
+      <c r="J140" t="s">
+        <v>668</v>
+      </c>
+      <c r="K140" t="b">
         <v>0</v>
       </c>
-      <c r="I140" t="s">
+      <c r="L140" t="s">
         <v>596</v>
       </c>
-      <c r="J140" t="s">
+      <c r="M140" t="s">
         <v>596</v>
       </c>
-      <c r="K140" t="s">
+      <c r="N140" t="s">
         <v>603</v>
       </c>
     </row>
-    <row r="141" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
         <v>588</v>
       </c>
@@ -6958,19 +8251,28 @@
         <v>11</v>
       </c>
       <c r="H141" t="b">
+        <v>1</v>
+      </c>
+      <c r="I141" t="b">
+        <v>1</v>
+      </c>
+      <c r="J141" t="s">
+        <v>668</v>
+      </c>
+      <c r="K141" t="b">
         <v>0</v>
       </c>
-      <c r="I141" t="s">
+      <c r="L141" t="s">
         <v>597</v>
       </c>
-      <c r="J141" t="s">
+      <c r="M141" t="s">
         <v>597</v>
       </c>
-      <c r="K141">
+      <c r="N141">
         <v>1.2</v>
       </c>
     </row>
-    <row r="142" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B142" t="s">
         <v>589</v>
       </c>
@@ -6987,19 +8289,28 @@
         <v>104</v>
       </c>
       <c r="H142" t="b">
+        <v>1</v>
+      </c>
+      <c r="I142" t="b">
+        <v>1</v>
+      </c>
+      <c r="J142" t="s">
+        <v>668</v>
+      </c>
+      <c r="K142" t="b">
         <v>0</v>
       </c>
-      <c r="I142" t="s">
+      <c r="L142" t="s">
         <v>592</v>
       </c>
-      <c r="J142" t="s">
+      <c r="M142" t="s">
         <v>650</v>
       </c>
-      <c r="K142" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="143" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="N142" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B143" t="s">
         <v>598</v>
       </c>
@@ -7016,20 +8327,29 @@
         <v>11</v>
       </c>
       <c r="H143" t="b">
+        <v>1</v>
+      </c>
+      <c r="I143" t="b">
+        <v>1</v>
+      </c>
+      <c r="J143" t="s">
+        <v>667</v>
+      </c>
+      <c r="K143" t="b">
         <v>0</v>
       </c>
-      <c r="I143" t="s">
+      <c r="L143" t="s">
         <v>599</v>
       </c>
-      <c r="J143" t="s">
+      <c r="M143" t="s">
         <v>651</v>
       </c>
-      <c r="K143" t="s">
+      <c r="N143" t="s">
         <v>604</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L143" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:O143" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix reports and filters
</commit_message>
<xml_diff>
--- a/db/airr_schema_defs.xlsx
+++ b/db/airr_schema_defs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Research\digby_backend\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1358572-622C-48DE-8EF2-D039B9BA9326}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AA75DE1-6F1E-43FB-8F02-59AAADDCE91E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="airr_schema_defs" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">airr_schema_defs!$A$1:$P$144</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">airr_schema_defs!$A$1:$Q$144</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1273" uniqueCount="685">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1274" uniqueCount="685">
   <si>
     <t>structured_name</t>
   </si>
@@ -2094,9 +2094,6 @@
     <t>Links to haplotype reports</t>
   </si>
   <si>
-    <t>genotypes</t>
-  </si>
-  <si>
     <t>haplotypes</t>
   </si>
   <si>
@@ -2107,6 +2104,9 @@
   </si>
   <si>
     <t>order</t>
+  </si>
+  <si>
+    <t>bool_value</t>
   </si>
 </sst>
 </file>
@@ -2959,10 +2959,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P144"/>
+  <dimension ref="A1:Q144"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2972,12 +2972,12 @@
     <col min="3" max="4" width="27.140625" customWidth="1"/>
     <col min="5" max="5" width="28" customWidth="1"/>
     <col min="6" max="6" width="39.28515625" customWidth="1"/>
-    <col min="13" max="13" width="35.42578125" customWidth="1"/>
-    <col min="14" max="14" width="148.28515625" customWidth="1"/>
-    <col min="15" max="15" width="58.42578125" customWidth="1"/>
+    <col min="13" max="14" width="35.42578125" customWidth="1"/>
+    <col min="15" max="15" width="148.28515625" customWidth="1"/>
+    <col min="16" max="16" width="58.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3003,7 +3003,7 @@
         <v>650</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>651</v>
@@ -3018,16 +3018,19 @@
         <v>5</v>
       </c>
       <c r="N1" s="3" t="s">
+        <v>684</v>
+      </c>
+      <c r="O1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>531</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -3058,11 +3061,11 @@
       <c r="M2" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -3093,11 +3096,11 @@
       <c r="M3" t="s">
         <v>16</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -3128,11 +3131,11 @@
       <c r="M4" t="s">
         <v>20</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -3172,14 +3175,14 @@
       <c r="M5" t="s">
         <v>25</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>26</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -3210,14 +3213,14 @@
       <c r="M6" t="s">
         <v>30</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>31</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -3248,11 +3251,11 @@
       <c r="M7" t="s">
         <v>660</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -3283,11 +3286,11 @@
       <c r="M8" t="s">
         <v>35</v>
       </c>
-      <c r="N8" t="s">
+      <c r="O8" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -3318,14 +3321,14 @@
       <c r="M9" t="s">
         <v>42</v>
       </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
         <v>43</v>
       </c>
-      <c r="O9" t="s">
+      <c r="P9" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -3356,14 +3359,14 @@
       <c r="M10" t="s">
         <v>665</v>
       </c>
-      <c r="N10" t="s">
+      <c r="O10" t="s">
         <v>47</v>
       </c>
-      <c r="O10" t="s">
+      <c r="P10" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -3394,14 +3397,14 @@
       <c r="M11" t="s">
         <v>51</v>
       </c>
-      <c r="N11" t="s">
+      <c r="O11" t="s">
         <v>52</v>
       </c>
-      <c r="O11" t="s">
+      <c r="P11" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>54</v>
       </c>
@@ -3438,14 +3441,14 @@
       <c r="M12" t="s">
         <v>56</v>
       </c>
-      <c r="N12" s="1" t="s">
+      <c r="O12" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="O12" t="s">
+      <c r="P12" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>59</v>
       </c>
@@ -3476,14 +3479,14 @@
       <c r="M13" t="s">
         <v>666</v>
       </c>
-      <c r="N13" s="1" t="s">
+      <c r="O13" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="O13" t="s">
+      <c r="P13" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -3517,14 +3520,14 @@
       <c r="M14" t="s">
         <v>65</v>
       </c>
-      <c r="N14" t="s">
+      <c r="O14" t="s">
         <v>66</v>
       </c>
-      <c r="O14" t="s">
+      <c r="P14" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>68</v>
       </c>
@@ -3561,14 +3564,14 @@
       <c r="M15" t="s">
         <v>70</v>
       </c>
-      <c r="N15" t="s">
+      <c r="O15" t="s">
         <v>71</v>
       </c>
-      <c r="O15" t="s">
+      <c r="P15" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>73</v>
       </c>
@@ -3605,14 +3608,14 @@
       <c r="M16" t="s">
         <v>667</v>
       </c>
-      <c r="N16" s="1" t="s">
+      <c r="O16" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="O16" t="s">
+      <c r="P16" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -3649,14 +3652,14 @@
       <c r="M17" t="s">
         <v>79</v>
       </c>
-      <c r="N17" t="s">
+      <c r="O17" t="s">
         <v>80</v>
       </c>
-      <c r="O17" t="s">
+      <c r="P17" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>82</v>
       </c>
@@ -3688,7 +3691,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>85</v>
       </c>
@@ -3719,14 +3722,14 @@
       <c r="M19" t="s">
         <v>87</v>
       </c>
-      <c r="N19" s="1" t="s">
+      <c r="O19" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O19" s="2">
+      <c r="P19" s="2">
         <v>44229</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>89</v>
       </c>
@@ -3757,14 +3760,14 @@
       <c r="M20" t="s">
         <v>91</v>
       </c>
-      <c r="N20" s="1" t="s">
+      <c r="O20" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="O20" s="2">
+      <c r="P20" s="2">
         <v>44229</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>93</v>
       </c>
@@ -3801,14 +3804,14 @@
       <c r="M21" t="s">
         <v>96</v>
       </c>
-      <c r="N21" t="s">
+      <c r="O21" t="s">
         <v>97</v>
       </c>
-      <c r="O21" t="s">
+      <c r="P21" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>99</v>
       </c>
@@ -3839,11 +3842,11 @@
       <c r="M22" t="s">
         <v>102</v>
       </c>
-      <c r="N22" t="s">
+      <c r="O22" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>104</v>
       </c>
@@ -3874,11 +3877,11 @@
       <c r="M23" t="s">
         <v>661</v>
       </c>
-      <c r="N23" t="s">
+      <c r="O23" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>107</v>
       </c>
@@ -3909,11 +3912,11 @@
       <c r="M24" t="s">
         <v>662</v>
       </c>
-      <c r="N24" t="s">
+      <c r="O24" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>109</v>
       </c>
@@ -3944,11 +3947,11 @@
       <c r="M25" t="s">
         <v>655</v>
       </c>
-      <c r="N25" t="s">
+      <c r="O25" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>111</v>
       </c>
@@ -3979,11 +3982,11 @@
       <c r="M26" t="s">
         <v>106</v>
       </c>
-      <c r="N26" t="s">
+      <c r="O26" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>113</v>
       </c>
@@ -4020,14 +4023,14 @@
       <c r="M27" t="s">
         <v>115</v>
       </c>
-      <c r="N27" t="s">
+      <c r="O27" t="s">
         <v>116</v>
       </c>
-      <c r="O27" t="s">
+      <c r="P27" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>118</v>
       </c>
@@ -4058,14 +4061,14 @@
       <c r="M28" t="s">
         <v>120</v>
       </c>
-      <c r="N28" t="s">
+      <c r="O28" t="s">
         <v>121</v>
       </c>
-      <c r="O28">
+      <c r="P28">
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>122</v>
       </c>
@@ -4096,14 +4099,14 @@
       <c r="M29" t="s">
         <v>124</v>
       </c>
-      <c r="N29" s="1" t="s">
+      <c r="O29" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="O29">
+      <c r="P29">
         <v>80</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>126</v>
       </c>
@@ -4134,11 +4137,11 @@
       <c r="M30" t="s">
         <v>663</v>
       </c>
-      <c r="N30" t="s">
+      <c r="O30" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>129</v>
       </c>
@@ -4169,11 +4172,11 @@
       <c r="M31" t="s">
         <v>128</v>
       </c>
-      <c r="N31" t="s">
+      <c r="O31" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>131</v>
       </c>
@@ -4204,14 +4207,14 @@
       <c r="M32" t="s">
         <v>133</v>
       </c>
-      <c r="N32" s="1" t="s">
+      <c r="O32" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="O32" t="s">
+      <c r="P32" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>136</v>
       </c>
@@ -4249,7 +4252,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>138</v>
       </c>
@@ -4286,14 +4289,14 @@
       <c r="M34" t="s">
         <v>140</v>
       </c>
-      <c r="N34" t="s">
+      <c r="O34" t="s">
         <v>141</v>
       </c>
-      <c r="O34" t="s">
+      <c r="P34" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>143</v>
       </c>
@@ -4330,14 +4333,14 @@
       <c r="M35" t="s">
         <v>145</v>
       </c>
-      <c r="N35" t="s">
+      <c r="O35" t="s">
         <v>146</v>
       </c>
-      <c r="O35" t="s">
+      <c r="P35" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>148</v>
       </c>
@@ -4368,14 +4371,14 @@
       <c r="M36" t="s">
         <v>150</v>
       </c>
-      <c r="N36" t="s">
+      <c r="O36" t="s">
         <v>151</v>
       </c>
-      <c r="O36" t="s">
+      <c r="P36" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>153</v>
       </c>
@@ -4406,14 +4409,14 @@
       <c r="M37" t="s">
         <v>155</v>
       </c>
-      <c r="N37" t="s">
+      <c r="O37" t="s">
         <v>156</v>
       </c>
-      <c r="O37" t="s">
+      <c r="P37" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>158</v>
       </c>
@@ -4444,14 +4447,14 @@
       <c r="M38" t="s">
         <v>160</v>
       </c>
-      <c r="N38" t="s">
+      <c r="O38" t="s">
         <v>161</v>
       </c>
-      <c r="O38" t="s">
+      <c r="P38" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>163</v>
       </c>
@@ -4482,14 +4485,14 @@
       <c r="M39" t="s">
         <v>165</v>
       </c>
-      <c r="N39" t="s">
+      <c r="O39" t="s">
         <v>166</v>
       </c>
-      <c r="O39" t="s">
+      <c r="P39" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>168</v>
       </c>
@@ -4526,14 +4529,14 @@
       <c r="M40" t="s">
         <v>170</v>
       </c>
-      <c r="N40" t="s">
+      <c r="O40" t="s">
         <v>171</v>
       </c>
-      <c r="O40" t="s">
+      <c r="P40" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>173</v>
       </c>
@@ -4564,11 +4567,11 @@
       <c r="M41" t="s">
         <v>175</v>
       </c>
-      <c r="N41" t="s">
+      <c r="O41" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>176</v>
       </c>
@@ -4605,11 +4608,11 @@
       <c r="M42" t="s">
         <v>175</v>
       </c>
-      <c r="N42" t="s">
+      <c r="O42" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>178</v>
       </c>
@@ -4640,14 +4643,14 @@
       <c r="M43" t="s">
         <v>180</v>
       </c>
-      <c r="N43" t="s">
+      <c r="O43" t="s">
         <v>181</v>
       </c>
-      <c r="O43" t="s">
+      <c r="P43" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>183</v>
       </c>
@@ -4678,14 +4681,14 @@
       <c r="M44" t="s">
         <v>185</v>
       </c>
-      <c r="N44" t="s">
+      <c r="O44" t="s">
         <v>186</v>
       </c>
-      <c r="O44" t="s">
+      <c r="P44" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>188</v>
       </c>
@@ -4716,14 +4719,14 @@
       <c r="M45" t="s">
         <v>668</v>
       </c>
-      <c r="N45" t="s">
+      <c r="O45" t="s">
         <v>190</v>
       </c>
-      <c r="O45" t="s">
+      <c r="P45" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>192</v>
       </c>
@@ -4754,14 +4757,14 @@
       <c r="M46" t="s">
         <v>194</v>
       </c>
-      <c r="N46" t="s">
+      <c r="O46" t="s">
         <v>195</v>
       </c>
-      <c r="O46" t="s">
+      <c r="P46" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>197</v>
       </c>
@@ -4792,14 +4795,14 @@
       <c r="M47" t="s">
         <v>199</v>
       </c>
-      <c r="N47" t="s">
+      <c r="O47" t="s">
         <v>200</v>
       </c>
-      <c r="O47" t="s">
+      <c r="P47" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>202</v>
       </c>
@@ -4830,14 +4833,14 @@
       <c r="M48" t="s">
         <v>204</v>
       </c>
-      <c r="N48" t="s">
+      <c r="O48" t="s">
         <v>205</v>
       </c>
-      <c r="O48" t="s">
+      <c r="P48" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>207</v>
       </c>
@@ -4865,11 +4868,11 @@
       <c r="L49" t="b">
         <v>0</v>
       </c>
-      <c r="N49" t="s">
+      <c r="O49" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>210</v>
       </c>
@@ -4897,11 +4900,11 @@
       <c r="L50" t="b">
         <v>0</v>
       </c>
-      <c r="N50" t="s">
+      <c r="O50" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>213</v>
       </c>
@@ -4929,11 +4932,11 @@
       <c r="L51" t="b">
         <v>1</v>
       </c>
-      <c r="N51" t="s">
+      <c r="O51" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>216</v>
       </c>
@@ -4961,11 +4964,11 @@
       <c r="L52" t="b">
         <v>1</v>
       </c>
-      <c r="O52" t="s">
+      <c r="P52" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>219</v>
       </c>
@@ -4993,11 +4996,11 @@
       <c r="L53" t="b">
         <v>1</v>
       </c>
-      <c r="N53" t="s">
+      <c r="O53" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>222</v>
       </c>
@@ -5025,11 +5028,11 @@
       <c r="L54" t="b">
         <v>1</v>
       </c>
-      <c r="N54" t="s">
+      <c r="O54" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>225</v>
       </c>
@@ -5060,14 +5063,14 @@
       <c r="M55" t="s">
         <v>227</v>
       </c>
-      <c r="N55" t="s">
+      <c r="O55" t="s">
         <v>228</v>
       </c>
-      <c r="O55" t="s">
+      <c r="P55" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="56" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>230</v>
       </c>
@@ -5098,11 +5101,11 @@
       <c r="M56" t="s">
         <v>233</v>
       </c>
-      <c r="N56" s="1" t="s">
+      <c r="O56" s="1" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>235</v>
       </c>
@@ -5133,14 +5136,14 @@
       <c r="M57" t="s">
         <v>238</v>
       </c>
-      <c r="N57" t="s">
+      <c r="O57" t="s">
         <v>239</v>
       </c>
-      <c r="O57" t="s">
+      <c r="P57" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>241</v>
       </c>
@@ -5171,14 +5174,14 @@
       <c r="M58" t="s">
         <v>243</v>
       </c>
-      <c r="N58" t="s">
+      <c r="O58" t="s">
         <v>244</v>
       </c>
-      <c r="O58" t="s">
+      <c r="P58" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>246</v>
       </c>
@@ -5197,11 +5200,8 @@
       <c r="H59" t="b">
         <v>1</v>
       </c>
-      <c r="I59">
-        <v>5</v>
-      </c>
       <c r="J59" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K59" t="s">
         <v>653</v>
@@ -5212,11 +5212,11 @@
       <c r="M59" t="s">
         <v>664</v>
       </c>
-      <c r="N59" t="s">
+      <c r="O59" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>249</v>
       </c>
@@ -5241,8 +5241,11 @@
       <c r="H60" t="b">
         <v>1</v>
       </c>
+      <c r="I60">
+        <v>5</v>
+      </c>
       <c r="J60" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K60" t="s">
         <v>653</v>
@@ -5253,11 +5256,11 @@
       <c r="M60" t="s">
         <v>248</v>
       </c>
-      <c r="N60" t="s">
+      <c r="O60" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>251</v>
       </c>
@@ -5288,14 +5291,14 @@
       <c r="M61" t="s">
         <v>253</v>
       </c>
-      <c r="N61" t="s">
+      <c r="O61" t="s">
         <v>254</v>
       </c>
-      <c r="O61" t="s">
+      <c r="P61" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>256</v>
       </c>
@@ -5326,14 +5329,14 @@
       <c r="M62" t="s">
         <v>258</v>
       </c>
-      <c r="N62" t="s">
+      <c r="O62" t="s">
         <v>259</v>
       </c>
-      <c r="O62" t="s">
+      <c r="P62" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>261</v>
       </c>
@@ -5367,14 +5370,14 @@
       <c r="M63" t="s">
         <v>263</v>
       </c>
-      <c r="N63" t="s">
+      <c r="O63" t="s">
         <v>264</v>
       </c>
-      <c r="O63">
+      <c r="P63">
         <v>14</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>265</v>
       </c>
@@ -5405,11 +5408,11 @@
       <c r="M64" t="s">
         <v>267</v>
       </c>
-      <c r="N64" t="s">
+      <c r="O64" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>268</v>
       </c>
@@ -5440,11 +5443,11 @@
       <c r="M65" t="s">
         <v>267</v>
       </c>
-      <c r="N65" t="s">
+      <c r="O65" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>270</v>
       </c>
@@ -5475,14 +5478,14 @@
       <c r="M66" t="s">
         <v>272</v>
       </c>
-      <c r="N66" t="s">
+      <c r="O66" t="s">
         <v>273</v>
       </c>
-      <c r="O66" t="s">
+      <c r="P66" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>275</v>
       </c>
@@ -5513,14 +5516,14 @@
       <c r="M67" t="s">
         <v>277</v>
       </c>
-      <c r="N67" t="s">
+      <c r="O67" t="s">
         <v>278</v>
       </c>
-      <c r="O67" t="s">
+      <c r="P67" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>280</v>
       </c>
@@ -5554,14 +5557,14 @@
       <c r="M68" t="s">
         <v>283</v>
       </c>
-      <c r="N68" t="s">
+      <c r="O68" t="s">
         <v>284</v>
       </c>
-      <c r="O68" t="s">
+      <c r="P68" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>286</v>
       </c>
@@ -5592,11 +5595,11 @@
       <c r="M69" t="s">
         <v>658</v>
       </c>
-      <c r="N69" t="s">
+      <c r="O69" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>289</v>
       </c>
@@ -5633,11 +5636,11 @@
       <c r="M70" t="s">
         <v>288</v>
       </c>
-      <c r="N70" t="s">
+      <c r="O70" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>291</v>
       </c>
@@ -5674,14 +5677,14 @@
       <c r="M71" t="s">
         <v>293</v>
       </c>
-      <c r="N71" t="s">
+      <c r="O71" t="s">
         <v>294</v>
       </c>
-      <c r="O71" t="s">
+      <c r="P71" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>296</v>
       </c>
@@ -5712,11 +5715,11 @@
       <c r="M72" t="s">
         <v>659</v>
       </c>
-      <c r="N72" t="s">
+      <c r="O72" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>299</v>
       </c>
@@ -5753,11 +5756,11 @@
       <c r="M73" t="s">
         <v>298</v>
       </c>
-      <c r="N73" t="s">
+      <c r="O73" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>301</v>
       </c>
@@ -5788,11 +5791,11 @@
       <c r="M74" t="s">
         <v>303</v>
       </c>
-      <c r="N74" t="s">
+      <c r="O74" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>305</v>
       </c>
@@ -5823,14 +5826,14 @@
       <c r="M75" t="s">
         <v>308</v>
       </c>
-      <c r="N75" t="s">
+      <c r="O75" t="s">
         <v>309</v>
       </c>
-      <c r="O75">
+      <c r="P75">
         <v>1000000</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>310</v>
       </c>
@@ -5861,14 +5864,14 @@
       <c r="M76" t="s">
         <v>669</v>
       </c>
-      <c r="N76" t="s">
+      <c r="O76" t="s">
         <v>312</v>
       </c>
-      <c r="O76">
+      <c r="P76">
         <v>50000</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>313</v>
       </c>
@@ -5899,14 +5902,14 @@
       <c r="M77" t="s">
         <v>315</v>
       </c>
-      <c r="N77" t="s">
+      <c r="O77" t="s">
         <v>316</v>
       </c>
-      <c r="O77" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P77" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>317</v>
       </c>
@@ -5937,14 +5940,14 @@
       <c r="M78" t="s">
         <v>319</v>
       </c>
-      <c r="N78" t="s">
+      <c r="O78" t="s">
         <v>320</v>
       </c>
-      <c r="O78" t="s">
+      <c r="P78" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="79" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>322</v>
       </c>
@@ -5975,14 +5978,14 @@
       <c r="M79" t="s">
         <v>675</v>
       </c>
-      <c r="N79" t="s">
+      <c r="O79" t="s">
         <v>324</v>
       </c>
-      <c r="O79" s="1" t="s">
+      <c r="P79" s="1" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="80" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>326</v>
       </c>
@@ -6013,14 +6016,14 @@
       <c r="M80" t="s">
         <v>328</v>
       </c>
-      <c r="N80" s="1" t="s">
+      <c r="O80" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="O80" t="s">
+      <c r="P80" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="81" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>331</v>
       </c>
@@ -6057,14 +6060,14 @@
       <c r="M81" t="s">
         <v>334</v>
       </c>
-      <c r="N81" s="1" t="s">
+      <c r="O81" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="O81" t="s">
+      <c r="P81" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>337</v>
       </c>
@@ -6095,14 +6098,14 @@
       <c r="M82" t="s">
         <v>339</v>
       </c>
-      <c r="N82" t="s">
+      <c r="O82" t="s">
         <v>340</v>
       </c>
-      <c r="O82" t="s">
+      <c r="P82" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>342</v>
       </c>
@@ -6133,14 +6136,14 @@
       <c r="M83" t="s">
         <v>344</v>
       </c>
-      <c r="N83" t="s">
+      <c r="O83" t="s">
         <v>345</v>
       </c>
-      <c r="O83">
+      <c r="P83">
         <v>1000</v>
       </c>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>346</v>
       </c>
@@ -6169,13 +6172,13 @@
         <v>1</v>
       </c>
       <c r="M84" t="s">
-        <v>682</v>
-      </c>
-      <c r="N84" t="s">
+        <v>681</v>
+      </c>
+      <c r="O84" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>348</v>
       </c>
@@ -6204,13 +6207,13 @@
         <v>1</v>
       </c>
       <c r="M85" t="s">
-        <v>683</v>
-      </c>
-      <c r="N85" t="s">
+        <v>682</v>
+      </c>
+      <c r="O85" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>350</v>
       </c>
@@ -6247,14 +6250,14 @@
       <c r="M86" t="s">
         <v>352</v>
       </c>
-      <c r="N86" t="s">
+      <c r="O86" t="s">
         <v>353</v>
       </c>
-      <c r="O86" t="s">
+      <c r="P86" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>355</v>
       </c>
@@ -6285,14 +6288,14 @@
       <c r="M87" t="s">
         <v>357</v>
       </c>
-      <c r="N87" t="s">
+      <c r="O87" t="s">
         <v>358</v>
       </c>
-      <c r="O87" t="s">
+      <c r="P87" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>360</v>
       </c>
@@ -6323,14 +6326,14 @@
       <c r="M88" t="s">
         <v>362</v>
       </c>
-      <c r="N88" t="s">
+      <c r="O88" t="s">
         <v>363</v>
       </c>
-      <c r="O88" t="s">
+      <c r="P88" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="89" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>365</v>
       </c>
@@ -6367,14 +6370,14 @@
       <c r="M89" t="s">
         <v>367</v>
       </c>
-      <c r="N89" s="1" t="s">
+      <c r="O89" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="O89" t="s">
+      <c r="P89" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>370</v>
       </c>
@@ -6411,14 +6414,14 @@
       <c r="M90" t="s">
         <v>670</v>
       </c>
-      <c r="N90" t="s">
+      <c r="O90" t="s">
         <v>372</v>
       </c>
-      <c r="O90" t="s">
+      <c r="P90" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>374</v>
       </c>
@@ -6455,14 +6458,14 @@
       <c r="M91" t="s">
         <v>671</v>
       </c>
-      <c r="N91" t="s">
+      <c r="O91" t="s">
         <v>376</v>
       </c>
-      <c r="O91" t="s">
+      <c r="P91" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="92" spans="1:15" ht="105" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:16" ht="105" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>378</v>
       </c>
@@ -6496,14 +6499,14 @@
       <c r="M92" t="s">
         <v>380</v>
       </c>
-      <c r="N92" s="1" t="s">
+      <c r="O92" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="O92" t="s">
+      <c r="P92" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="93" spans="1:15" ht="90" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:16" ht="90" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>383</v>
       </c>
@@ -6534,14 +6537,14 @@
       <c r="M93" t="s">
         <v>672</v>
       </c>
-      <c r="N93" s="1" t="s">
+      <c r="O93" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="O93" t="s">
+      <c r="P93" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>387</v>
       </c>
@@ -6572,14 +6575,14 @@
       <c r="M94" t="s">
         <v>390</v>
       </c>
-      <c r="N94" t="s">
+      <c r="O94" t="s">
         <v>391</v>
       </c>
-      <c r="O94" t="s">
+      <c r="P94" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>393</v>
       </c>
@@ -6610,14 +6613,14 @@
       <c r="M95" t="s">
         <v>395</v>
       </c>
-      <c r="N95" t="s">
+      <c r="O95" t="s">
         <v>396</v>
       </c>
-      <c r="O95">
+      <c r="P95">
         <v>10365118</v>
       </c>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>397</v>
       </c>
@@ -6654,14 +6657,14 @@
       <c r="M96" t="s">
         <v>399</v>
       </c>
-      <c r="N96" t="s">
+      <c r="O96" t="s">
         <v>400</v>
       </c>
-      <c r="O96" t="s">
+      <c r="P96" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>402</v>
       </c>
@@ -6692,14 +6695,14 @@
       <c r="M97" t="s">
         <v>404</v>
       </c>
-      <c r="N97" t="s">
+      <c r="O97" t="s">
         <v>405</v>
       </c>
-      <c r="O97" t="s">
+      <c r="P97" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>407</v>
       </c>
@@ -6730,14 +6733,14 @@
       <c r="M98" t="s">
         <v>409</v>
       </c>
-      <c r="N98" t="s">
+      <c r="O98" t="s">
         <v>409</v>
       </c>
-      <c r="O98" s="2">
+      <c r="P98" s="2">
         <v>42720</v>
       </c>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>410</v>
       </c>
@@ -6768,14 +6771,14 @@
       <c r="M99" t="s">
         <v>412</v>
       </c>
-      <c r="N99" t="s">
+      <c r="O99" t="s">
         <v>413</v>
       </c>
-      <c r="O99" t="s">
+      <c r="P99" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>415</v>
       </c>
@@ -6806,11 +6809,11 @@
       <c r="M100" t="s">
         <v>417</v>
       </c>
-      <c r="N100" t="s">
+      <c r="O100" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>419</v>
       </c>
@@ -6841,14 +6844,14 @@
       <c r="M101" t="s">
         <v>421</v>
       </c>
-      <c r="N101" t="s">
+      <c r="O101" t="s">
         <v>422</v>
       </c>
-      <c r="O101" t="s">
+      <c r="P101" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>424</v>
       </c>
@@ -6879,14 +6882,14 @@
       <c r="M102" t="s">
         <v>426</v>
       </c>
-      <c r="N102" t="s">
+      <c r="O102" t="s">
         <v>427</v>
       </c>
-      <c r="O102" t="s">
+      <c r="P102" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>429</v>
       </c>
@@ -6923,14 +6926,14 @@
       <c r="M103" t="s">
         <v>431</v>
       </c>
-      <c r="N103" t="s">
+      <c r="O103" t="s">
         <v>432</v>
       </c>
-      <c r="O103">
+      <c r="P103">
         <v>300</v>
       </c>
     </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>433</v>
       </c>
@@ -6961,14 +6964,14 @@
       <c r="M104" t="s">
         <v>657</v>
       </c>
-      <c r="N104" t="s">
+      <c r="O104" t="s">
         <v>435</v>
       </c>
-      <c r="O104" t="s">
+      <c r="P104" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>437</v>
       </c>
@@ -6999,14 +7002,14 @@
       <c r="M105" t="s">
         <v>439</v>
       </c>
-      <c r="N105" t="s">
+      <c r="O105" t="s">
         <v>440</v>
       </c>
-      <c r="O105" t="s">
+      <c r="P105" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>442</v>
       </c>
@@ -7037,14 +7040,14 @@
       <c r="M106" t="s">
         <v>444</v>
       </c>
-      <c r="N106" t="s">
+      <c r="O106" t="s">
         <v>445</v>
       </c>
-      <c r="O106">
+      <c r="P106">
         <v>300</v>
       </c>
     </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>446</v>
       </c>
@@ -7075,11 +7078,11 @@
       <c r="M107" t="s">
         <v>449</v>
       </c>
-      <c r="N107" t="s">
+      <c r="O107" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="108" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>451</v>
       </c>
@@ -7110,11 +7113,11 @@
       <c r="M108" t="s">
         <v>453</v>
       </c>
-      <c r="N108" s="1" t="s">
+      <c r="O108" s="1" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>455</v>
       </c>
@@ -7145,14 +7148,14 @@
       <c r="M109" t="s">
         <v>673</v>
       </c>
-      <c r="N109" t="s">
+      <c r="O109" t="s">
         <v>457</v>
       </c>
-      <c r="O109" t="s">
+      <c r="P109" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>459</v>
       </c>
@@ -7183,14 +7186,14 @@
       <c r="M110" t="s">
         <v>461</v>
       </c>
-      <c r="N110" t="s">
+      <c r="O110" t="s">
         <v>462</v>
       </c>
-      <c r="O110" t="s">
+      <c r="P110" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>464</v>
       </c>
@@ -7221,14 +7224,14 @@
       <c r="M111" t="s">
         <v>466</v>
       </c>
-      <c r="N111" t="s">
+      <c r="O111" t="s">
         <v>467</v>
       </c>
-      <c r="O111" t="s">
+      <c r="P111" t="s">
         <v>468</v>
       </c>
     </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>469</v>
       </c>
@@ -7259,14 +7262,14 @@
       <c r="M112" t="s">
         <v>471</v>
       </c>
-      <c r="N112" t="s">
+      <c r="O112" t="s">
         <v>472</v>
       </c>
-      <c r="O112" t="s">
+      <c r="P112" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="113" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>474</v>
       </c>
@@ -7297,14 +7300,14 @@
       <c r="M113" t="s">
         <v>476</v>
       </c>
-      <c r="N113" t="s">
+      <c r="O113" t="s">
         <v>477</v>
       </c>
-      <c r="O113" t="s">
+      <c r="P113" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>479</v>
       </c>
@@ -7335,14 +7338,14 @@
       <c r="M114" t="s">
         <v>481</v>
       </c>
-      <c r="N114" t="s">
+      <c r="O114" t="s">
         <v>482</v>
       </c>
-      <c r="O114" t="s">
+      <c r="P114" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="115" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>484</v>
       </c>
@@ -7374,7 +7377,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="116" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>487</v>
       </c>
@@ -7405,14 +7408,14 @@
       <c r="M116" t="s">
         <v>674</v>
       </c>
-      <c r="N116" t="s">
+      <c r="O116" t="s">
         <v>489</v>
       </c>
-      <c r="O116" t="s">
+      <c r="P116" t="s">
         <v>490</v>
       </c>
     </row>
-    <row r="117" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>491</v>
       </c>
@@ -7443,11 +7446,11 @@
       <c r="M117" t="s">
         <v>493</v>
       </c>
-      <c r="N117" t="s">
+      <c r="O117" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="118" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
         <v>532</v>
       </c>
@@ -7478,14 +7481,14 @@
       <c r="M118" t="s">
         <v>543</v>
       </c>
-      <c r="N118" t="s">
+      <c r="O118" t="s">
         <v>541</v>
       </c>
-      <c r="P118" t="s">
+      <c r="Q118" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
         <v>533</v>
       </c>
@@ -7516,14 +7519,14 @@
       <c r="M119" t="s">
         <v>544</v>
       </c>
-      <c r="N119" t="s">
+      <c r="O119" t="s">
         <v>542</v>
       </c>
-      <c r="P119" t="s">
+      <c r="Q119" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="120" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
         <v>534</v>
       </c>
@@ -7551,14 +7554,14 @@
       <c r="M120" t="s">
         <v>545</v>
       </c>
-      <c r="N120" s="1" t="s">
+      <c r="O120" s="1" t="s">
         <v>546</v>
       </c>
-      <c r="P120" t="s">
+      <c r="Q120" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="121" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
         <v>535</v>
       </c>
@@ -7589,14 +7592,14 @@
       <c r="M121" t="s">
         <v>547</v>
       </c>
-      <c r="N121" t="s">
+      <c r="O121" t="s">
         <v>548</v>
       </c>
-      <c r="P121" t="s">
+      <c r="Q121" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="122" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
         <v>647</v>
       </c>
@@ -7627,14 +7630,14 @@
       <c r="M122" t="s">
         <v>549</v>
       </c>
-      <c r="N122" t="s">
+      <c r="O122" t="s">
         <v>550</v>
       </c>
-      <c r="P122" t="s">
+      <c r="Q122" t="s">
         <v>516</v>
       </c>
     </row>
-    <row r="123" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
         <v>537</v>
       </c>
@@ -7662,14 +7665,14 @@
       <c r="M123" t="s">
         <v>551</v>
       </c>
-      <c r="N123" t="s">
+      <c r="O123" t="s">
         <v>552</v>
       </c>
-      <c r="P123" t="s">
+      <c r="Q123" t="s">
         <v>538</v>
       </c>
     </row>
-    <row r="124" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
         <v>649</v>
       </c>
@@ -7703,14 +7706,14 @@
       <c r="M124" t="s">
         <v>557</v>
       </c>
-      <c r="N124" t="s">
+      <c r="O124" t="s">
         <v>553</v>
       </c>
-      <c r="P124" t="s">
+      <c r="Q124" t="s">
         <v>516</v>
       </c>
     </row>
-    <row r="125" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
         <v>539</v>
       </c>
@@ -7744,16 +7747,16 @@
       <c r="M125" t="s">
         <v>634</v>
       </c>
-      <c r="N125" t="s">
+      <c r="O125" t="s">
         <v>635</v>
       </c>
-      <c r="P125" t="s">
+      <c r="Q125" t="s">
         <v>516</v>
       </c>
     </row>
-    <row r="126" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
-        <v>680</v>
+        <v>540</v>
       </c>
       <c r="D126" s="5" t="s">
         <v>237</v>
@@ -7782,16 +7785,16 @@
       <c r="M126" t="s">
         <v>554</v>
       </c>
-      <c r="N126" t="s">
+      <c r="O126" t="s">
         <v>678</v>
       </c>
-      <c r="P126" t="s">
+      <c r="Q126" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="127" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="D127" s="5" t="s">
         <v>237</v>
@@ -7820,11 +7823,11 @@
       <c r="M127" t="s">
         <v>677</v>
       </c>
-      <c r="N127" t="s">
+      <c r="O127" t="s">
         <v>679</v>
       </c>
     </row>
-    <row r="128" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
         <v>638</v>
       </c>
@@ -7852,11 +7855,11 @@
       <c r="M128" t="s">
         <v>639</v>
       </c>
-      <c r="N128" t="s">
+      <c r="O128" t="s">
         <v>640</v>
       </c>
     </row>
-    <row r="129" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
         <v>558</v>
       </c>
@@ -7887,14 +7890,14 @@
       <c r="M129" t="s">
         <v>555</v>
       </c>
-      <c r="N129" t="s">
+      <c r="O129" t="s">
         <v>555</v>
       </c>
-      <c r="P129" t="s">
+      <c r="Q129" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="130" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
         <v>641</v>
       </c>
@@ -7922,11 +7925,11 @@
       <c r="M130" t="s">
         <v>642</v>
       </c>
-      <c r="N130" t="s">
+      <c r="O130" t="s">
         <v>643</v>
       </c>
     </row>
-    <row r="131" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
         <v>644</v>
       </c>
@@ -7954,11 +7957,11 @@
       <c r="M131" t="s">
         <v>554</v>
       </c>
-      <c r="N131" t="s">
+      <c r="O131" t="s">
         <v>645</v>
       </c>
     </row>
-    <row r="132" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
         <v>648</v>
       </c>
@@ -7986,11 +7989,11 @@
       <c r="M132" t="s">
         <v>556</v>
       </c>
-      <c r="N132" t="s">
+      <c r="O132" t="s">
         <v>556</v>
       </c>
     </row>
-    <row r="133" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
         <v>568</v>
       </c>
@@ -8021,14 +8024,14 @@
       <c r="M133" t="s">
         <v>576</v>
       </c>
-      <c r="N133" t="s">
+      <c r="O133" t="s">
         <v>576</v>
       </c>
-      <c r="O133" t="s">
+      <c r="P133" t="s">
         <v>587</v>
       </c>
     </row>
-    <row r="134" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
         <v>569</v>
       </c>
@@ -8059,14 +8062,14 @@
       <c r="M134" t="s">
         <v>577</v>
       </c>
-      <c r="N134" t="s">
+      <c r="O134" t="s">
         <v>577</v>
       </c>
-      <c r="O134" t="s">
+      <c r="P134" t="s">
         <v>588</v>
       </c>
     </row>
-    <row r="135" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
         <v>570</v>
       </c>
@@ -8097,14 +8100,14 @@
       <c r="M135" t="s">
         <v>579</v>
       </c>
-      <c r="N135" t="s">
+      <c r="O135" t="s">
         <v>579</v>
       </c>
-      <c r="O135">
+      <c r="P135">
         <v>1.18</v>
       </c>
     </row>
-    <row r="136" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B136" t="s">
         <v>594</v>
       </c>
@@ -8135,14 +8138,14 @@
       <c r="M136" t="s">
         <v>629</v>
       </c>
-      <c r="N136" t="s">
+      <c r="O136" t="s">
         <v>629</v>
       </c>
-      <c r="O136" t="s">
+      <c r="P136" t="s">
         <v>628</v>
       </c>
     </row>
-    <row r="137" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
         <v>595</v>
       </c>
@@ -8173,14 +8176,14 @@
       <c r="M137" t="s">
         <v>630</v>
       </c>
-      <c r="N137" t="s">
+      <c r="O137" t="s">
         <v>630</v>
       </c>
-      <c r="O137" t="s">
+      <c r="P137" t="s">
         <v>628</v>
       </c>
     </row>
-    <row r="138" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B138" t="s">
         <v>596</v>
       </c>
@@ -8211,14 +8214,14 @@
       <c r="M138" t="s">
         <v>627</v>
       </c>
-      <c r="N138" t="s">
+      <c r="O138" t="s">
         <v>627</v>
       </c>
-      <c r="O138" t="s">
+      <c r="P138" t="s">
         <v>628</v>
       </c>
     </row>
-    <row r="139" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B139" t="s">
         <v>571</v>
       </c>
@@ -8249,14 +8252,14 @@
       <c r="M139" t="s">
         <v>580</v>
       </c>
-      <c r="N139" t="s">
+      <c r="O139" t="s">
         <v>580</v>
       </c>
-      <c r="O139" t="s">
+      <c r="P139" t="s">
         <v>586</v>
       </c>
     </row>
-    <row r="140" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
         <v>572</v>
       </c>
@@ -8287,14 +8290,14 @@
       <c r="M140" t="s">
         <v>581</v>
       </c>
-      <c r="N140" t="s">
+      <c r="O140" t="s">
         <v>581</v>
       </c>
-      <c r="O140">
+      <c r="P140">
         <v>1.2</v>
       </c>
     </row>
-    <row r="141" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
         <v>573</v>
       </c>
@@ -8325,14 +8328,14 @@
       <c r="M141" t="s">
         <v>582</v>
       </c>
-      <c r="N141" t="s">
+      <c r="O141" t="s">
         <v>582</v>
       </c>
-      <c r="O141" t="s">
+      <c r="P141" t="s">
         <v>589</v>
       </c>
     </row>
-    <row r="142" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B142" t="s">
         <v>574</v>
       </c>
@@ -8363,14 +8366,14 @@
       <c r="M142" t="s">
         <v>583</v>
       </c>
-      <c r="N142" t="s">
+      <c r="O142" t="s">
         <v>583</v>
       </c>
-      <c r="O142">
+      <c r="P142">
         <v>1.2</v>
       </c>
     </row>
-    <row r="143" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B143" t="s">
         <v>575</v>
       </c>
@@ -8401,14 +8404,14 @@
       <c r="M143" t="s">
         <v>578</v>
       </c>
-      <c r="N143" t="s">
+      <c r="O143" t="s">
         <v>636</v>
       </c>
-      <c r="O143" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="144" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="P143" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B144" t="s">
         <v>584</v>
       </c>
@@ -8439,10 +8442,10 @@
       <c r="M144" t="s">
         <v>585</v>
       </c>
-      <c r="N144" t="s">
+      <c r="O144" t="s">
         <v>637</v>
       </c>
-      <c r="O144" t="s">
+      <c r="P144" t="s">
         <v>590</v>
       </c>
     </row>

</xml_diff>

<commit_message>
More updates for miairr/yml take-on
</commit_message>
<xml_diff>
--- a/db/airr_schema_defs.xlsx
+++ b/db/airr_schema_defs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Research\digby_backend\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AA75DE1-6F1E-43FB-8F02-59AAADDCE91E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C35F251-84CB-4447-9B12-4E3BB631DB1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2962,7 +2962,7 @@
   <dimension ref="A1:Q144"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3505,11 +3505,8 @@
       <c r="H14" t="b">
         <v>1</v>
       </c>
-      <c r="I14">
-        <v>3</v>
-      </c>
       <c r="J14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K14" t="s">
         <v>654</v>
@@ -6478,6 +6475,12 @@
       <c r="D92" s="6" t="s">
         <v>529</v>
       </c>
+      <c r="E92" t="s">
+        <v>509</v>
+      </c>
+      <c r="F92" t="s">
+        <v>611</v>
+      </c>
       <c r="G92" t="s">
         <v>11</v>
       </c>
@@ -6901,12 +6904,6 @@
       </c>
       <c r="D103" s="6" t="s">
         <v>529</v>
-      </c>
-      <c r="E103" t="s">
-        <v>509</v>
-      </c>
-      <c r="F103" t="s">
-        <v>611</v>
       </c>
       <c r="G103" t="s">
         <v>307</v>

</xml_diff>